<commit_message>
Jan 2024 re release
</commit_message>
<xml_diff>
--- a/xlsx/funders.xlsx
+++ b/xlsx/funders.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emckclac-my.sharepoint.com/personal/k1780970_kcl_ac_uk/Documents/1. Catalogue + work documents/1. Catalogue shared files/1. Catalogue/2. Catalogue study updates/Funders files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Workspace/catalogue-mental-health/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{0F7304FC-427B-7E49-A9EE-3A29E7B8DC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40F1C249-5431-4231-9BF6-9C5FDE07DD39}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373C6AD9-7828-634F-87D3-A6ACB6B772BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="0" windowWidth="21000" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AMK$2</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="261">
   <si>
     <t>Logos saved</t>
   </si>
@@ -83,6 +89,18 @@
     <t>Chief Scientist Office (CSO) of the Scottish Government’s Health Directorates</t>
   </si>
   <si>
+    <t>Alzheimer's Society</t>
+  </si>
+  <si>
+    <t>AlzhSoc</t>
+  </si>
+  <si>
+    <t>https://www.alzheimers.org.uk/</t>
+  </si>
+  <si>
+    <t>International Centre for Child Studies</t>
+  </si>
+  <si>
     <t>American Asthma Foundation</t>
   </si>
   <si>
@@ -101,27 +119,27 @@
     <t>ARUK</t>
   </si>
   <si>
-    <t>https://www.versusarthritis.org/</t>
+    <t>https://www.arthritisresearchuk.org/</t>
   </si>
   <si>
     <t>Sir Siegmund Warburg Voluntary Settlement</t>
   </si>
   <si>
+    <t>Autism Speaks</t>
+  </si>
+  <si>
+    <t>AuSpeaks</t>
+  </si>
+  <si>
+    <t>https://www.autismspeaks.org/</t>
+  </si>
+  <si>
     <t>Autistica</t>
   </si>
   <si>
     <t>https://www.autistica.org.uk/</t>
   </si>
   <si>
-    <t>Autism Speaks</t>
-  </si>
-  <si>
-    <t>AuSpeaks</t>
-  </si>
-  <si>
-    <t>https://www.autismspeaks.org/</t>
-  </si>
-  <si>
     <t>Barrow Cadbury Trust</t>
   </si>
   <si>
@@ -140,9 +158,6 @@
     <t>https://www.tnlcommunityfund.org.uk/</t>
   </si>
   <si>
-    <t>International Centre for Child Studies</t>
-  </si>
-  <si>
     <t>Biotechnology and Biological Sciences Research Council</t>
   </si>
   <si>
@@ -152,6 +167,15 @@
     <t>https://bbsrc.ukri.org/</t>
   </si>
   <si>
+    <t>Blesma Limbless Veterans Charity</t>
+  </si>
+  <si>
+    <t>Blesma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://blesma.org/ </t>
+  </si>
+  <si>
     <t>British Heart Foundation</t>
   </si>
   <si>
@@ -197,6 +221,15 @@
     <t>https://www.cdrf.org.uk/</t>
   </si>
   <si>
+    <t>Department for Business, Energy &amp; Industrial Strategy</t>
+  </si>
+  <si>
+    <t>DBEIS</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/organisations/department-for-business-energy-and-industrial-strategy</t>
+  </si>
+  <si>
     <t>Department for Communities &amp; Local Government</t>
   </si>
   <si>
@@ -260,6 +293,15 @@
     <t>https://www.gov.uk/government/organisations/department-of-health-and-social-care</t>
   </si>
   <si>
+    <t>Dunhill Medical Trust</t>
+  </si>
+  <si>
+    <t>DMT</t>
+  </si>
+  <si>
+    <t>https://dunhillmedical.org.uk/</t>
+  </si>
+  <si>
     <t>Economic and Social Research Council</t>
   </si>
   <si>
@@ -269,6 +311,9 @@
     <t>https://esrc.ukri.org/</t>
   </si>
   <si>
+    <t>https://www.ukri.org/councils/esrc/</t>
+  </si>
+  <si>
     <t>European Commission</t>
   </si>
   <si>
@@ -314,13 +359,49 @@
     <t>https://www.food.gov.uk/</t>
   </si>
   <si>
+    <t>Forces in Mind Trust</t>
+  </si>
+  <si>
+    <t>FIMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.fim-trust.org/ </t>
+  </si>
+  <si>
     <t>German Federal Ministry of Education &amp; Research</t>
   </si>
   <si>
     <t>BMBF</t>
   </si>
   <si>
-    <t>https://www.bmbf.de/bmbf/en/home/home_node.html</t>
+    <t>https://www.bmbf.de/en/index.html</t>
+  </si>
+  <si>
+    <t>Guy's and St. Thomas' Charity</t>
+  </si>
+  <si>
+    <t>GSTT</t>
+  </si>
+  <si>
+    <t>https://gsttcharity.org.uk/</t>
+  </si>
+  <si>
+    <t>Help for Heroes</t>
+  </si>
+  <si>
+    <t>HFH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.helpforheroes.org.uk/ </t>
+  </si>
+  <si>
+    <t>Higher Education Funding Council for Wales</t>
+  </si>
+  <si>
+    <t>HEFCW</t>
+  </si>
+  <si>
+    <t>https://www.hefcw.ac.uk/en/</t>
   </si>
   <si>
     <t xml:space="preserve">Home Office </t>
@@ -347,7 +428,25 @@
     <t>https://research.hscni.net/</t>
   </si>
   <si>
-    <t>Innvative Medicines Initiative</t>
+    <t>Imperial College Biomedical Research Centre</t>
+  </si>
+  <si>
+    <t>Imperial_BRC</t>
+  </si>
+  <si>
+    <t>https://imperialbrc.nihr.ac.uk/</t>
+  </si>
+  <si>
+    <t>Imperial College Healthcare NHS Trust</t>
+  </si>
+  <si>
+    <t>ICNHS</t>
+  </si>
+  <si>
+    <t>https://www.imperial.nhs.uk/</t>
+  </si>
+  <si>
+    <t>Innovative Medicines Initiative</t>
   </si>
   <si>
     <t>IMI</t>
@@ -374,6 +473,15 @@
     <t>https://www.ukri.org/councils/mrc/</t>
   </si>
   <si>
+    <t>Ministry of Defence</t>
+  </si>
+  <si>
+    <t>MoD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.gov.uk/government/organisations/ministry-of-defence </t>
+  </si>
+  <si>
     <t>Ministry of Justice</t>
   </si>
   <si>
@@ -392,6 +500,12 @@
     <t>https://www.mqmentalhealth.org/</t>
   </si>
   <si>
+    <t>National Heart, Lung &amp; Blood Institute</t>
+  </si>
+  <si>
+    <t>https://www.nhlbi.nih.gov/</t>
+  </si>
+  <si>
     <t>National Institute for Health Research</t>
   </si>
   <si>
@@ -488,6 +602,15 @@
     <t>https://www.nuffieldfoundation.org/</t>
   </si>
   <si>
+    <t>Nuffield Trust for the Forces of the Crown</t>
+  </si>
+  <si>
+    <t>Nuffield_Crown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.nuffieldtrust.org/ </t>
+  </si>
+  <si>
     <t>Office for Veterans' Affairs</t>
   </si>
   <si>
@@ -563,6 +686,15 @@
     <t>https://www.gov.scot/</t>
   </si>
   <si>
+    <t>Seventh framework programme</t>
+  </si>
+  <si>
+    <t>FP7</t>
+  </si>
+  <si>
+    <t>https://cordis.europa.eu/programme/id/FP7/es</t>
+  </si>
+  <si>
     <t>Simons Foundation Autism Research Initative</t>
   </si>
   <si>
@@ -626,6 +758,15 @@
     <t>https://www.wolfson.org.uk/</t>
   </si>
   <si>
+    <t>UK Research and Innovation</t>
+  </si>
+  <si>
+    <t>UKRI</t>
+  </si>
+  <si>
+    <t>https://www.ukri.org/</t>
+  </si>
+  <si>
     <t>University of Bristol</t>
   </si>
   <si>
@@ -689,74 +830,14 @@
     <t>https://gov.wales/</t>
   </si>
   <si>
-    <t>Imperial College Healthcare NHS Trust</t>
-  </si>
-  <si>
-    <t>ICNHS</t>
-  </si>
-  <si>
-    <t>https://www.imperial.nhs.uk/</t>
-  </si>
-  <si>
-    <t>Imperial College Biomedical Research Centre</t>
-  </si>
-  <si>
-    <t>Imperial_BRC</t>
-  </si>
-  <si>
-    <t>https://imperialbrc.nihr.ac.uk/</t>
-  </si>
-  <si>
-    <t>Help for Heroes</t>
-  </si>
-  <si>
-    <t>HFH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.helpforheroes.org.uk/ </t>
-  </si>
-  <si>
-    <t>Nuffield Trust for the Forces of the Crown</t>
-  </si>
-  <si>
-    <t>Nuffield_Crown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.nuffieldtrust.org/ </t>
-  </si>
-  <si>
-    <t>Blesma Limbless Veterans Charity</t>
-  </si>
-  <si>
-    <t>Blesma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://blesma.org/ </t>
-  </si>
-  <si>
-    <t>Ministry of Defence</t>
-  </si>
-  <si>
-    <t>MoD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.gov.uk/government/organisations/ministry-of-defence </t>
-  </si>
-  <si>
-    <t>Forces in Mind Trust</t>
-  </si>
-  <si>
-    <t>FIMT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.fim-trust.org/ </t>
+    <t>NIH_Heart_Lung_Blood</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -812,12 +893,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -849,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -865,7 +940,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1249,25 +1323,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:AMK88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="51.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="51.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="1" customWidth="1"/>
-    <col min="5" max="5" width="60.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="60.83203125" style="1" customWidth="1"/>
     <col min="6" max="15" width="9" style="1" customWidth="1"/>
-    <col min="16" max="1025" width="8.42578125" style="1" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="1"/>
+    <col min="16" max="1025" width="8.5" style="1" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1277,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1291,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1305,7 +1379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1319,21 +1393,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1347,54 +1421,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="C9" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="C10" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1405,62 +1479,62 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -1471,29 +1545,29 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -1504,7 +1578,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
@@ -1515,7 +1589,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
@@ -1526,7 +1600,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -1537,7 +1611,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -1548,18 +1622,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
@@ -1570,293 +1644,1315 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="1" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15">
-      <c r="A30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="1" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="B31" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
+      <c r="C32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="33" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A33" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="4" t="s">
+    </row>
+    <row r="34" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="10" t="s">
+    </row>
+    <row r="35" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="5" t="s">
+    </row>
+    <row r="36" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="5" t="s">
+    </row>
+    <row r="37" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="4" t="s">
+    </row>
+    <row r="38" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+      <c r="AK38" s="7"/>
+      <c r="AL38" s="7"/>
+      <c r="AM38" s="7"/>
+      <c r="AN38" s="7"/>
+      <c r="AO38" s="7"/>
+      <c r="AP38" s="7"/>
+      <c r="AQ38" s="7"/>
+      <c r="AR38" s="7"/>
+      <c r="AS38" s="7"/>
+      <c r="AT38" s="7"/>
+      <c r="AU38" s="7"/>
+      <c r="AV38" s="7"/>
+      <c r="AW38" s="7"/>
+      <c r="AX38" s="7"/>
+      <c r="AY38" s="7"/>
+      <c r="AZ38" s="7"/>
+      <c r="BA38" s="7"/>
+      <c r="BB38" s="7"/>
+      <c r="BC38" s="7"/>
+      <c r="BD38" s="7"/>
+      <c r="BE38" s="7"/>
+      <c r="BF38" s="7"/>
+      <c r="BG38" s="7"/>
+      <c r="BH38" s="7"/>
+      <c r="BI38" s="7"/>
+      <c r="BJ38" s="7"/>
+      <c r="BK38" s="7"/>
+      <c r="BL38" s="7"/>
+      <c r="BM38" s="7"/>
+      <c r="BN38" s="7"/>
+      <c r="BO38" s="7"/>
+      <c r="BP38" s="7"/>
+      <c r="BQ38" s="7"/>
+      <c r="BR38" s="7"/>
+      <c r="BS38" s="7"/>
+      <c r="BT38" s="7"/>
+      <c r="BU38" s="7"/>
+      <c r="BV38" s="7"/>
+      <c r="BW38" s="7"/>
+      <c r="BX38" s="7"/>
+      <c r="BY38" s="7"/>
+      <c r="BZ38" s="7"/>
+      <c r="CA38" s="7"/>
+      <c r="CB38" s="7"/>
+      <c r="CC38" s="7"/>
+      <c r="CD38" s="7"/>
+      <c r="CE38" s="7"/>
+      <c r="CF38" s="7"/>
+      <c r="CG38" s="7"/>
+      <c r="CH38" s="7"/>
+      <c r="CI38" s="7"/>
+      <c r="CJ38" s="7"/>
+      <c r="CK38" s="7"/>
+      <c r="CL38" s="7"/>
+      <c r="CM38" s="7"/>
+      <c r="CN38" s="7"/>
+      <c r="CO38" s="7"/>
+      <c r="CP38" s="7"/>
+      <c r="CQ38" s="7"/>
+      <c r="CR38" s="7"/>
+      <c r="CS38" s="7"/>
+      <c r="CT38" s="7"/>
+      <c r="CU38" s="7"/>
+      <c r="CV38" s="7"/>
+      <c r="CW38" s="7"/>
+      <c r="CX38" s="7"/>
+      <c r="CY38" s="7"/>
+      <c r="CZ38" s="7"/>
+      <c r="DA38" s="7"/>
+      <c r="DB38" s="7"/>
+      <c r="DC38" s="7"/>
+      <c r="DD38" s="7"/>
+      <c r="DE38" s="7"/>
+      <c r="DF38" s="7"/>
+      <c r="DG38" s="7"/>
+      <c r="DH38" s="7"/>
+      <c r="DI38" s="7"/>
+      <c r="DJ38" s="7"/>
+      <c r="DK38" s="7"/>
+      <c r="DL38" s="7"/>
+      <c r="DM38" s="7"/>
+      <c r="DN38" s="7"/>
+      <c r="DO38" s="7"/>
+      <c r="DP38" s="7"/>
+      <c r="DQ38" s="7"/>
+      <c r="DR38" s="7"/>
+      <c r="DS38" s="7"/>
+      <c r="DT38" s="7"/>
+      <c r="DU38" s="7"/>
+      <c r="DV38" s="7"/>
+      <c r="DW38" s="7"/>
+      <c r="DX38" s="7"/>
+      <c r="DY38" s="7"/>
+      <c r="DZ38" s="7"/>
+      <c r="EA38" s="7"/>
+      <c r="EB38" s="7"/>
+      <c r="EC38" s="7"/>
+      <c r="ED38" s="7"/>
+      <c r="EE38" s="7"/>
+      <c r="EF38" s="7"/>
+      <c r="EG38" s="7"/>
+      <c r="EH38" s="7"/>
+      <c r="EI38" s="7"/>
+      <c r="EJ38" s="7"/>
+      <c r="EK38" s="7"/>
+      <c r="EL38" s="7"/>
+      <c r="EM38" s="7"/>
+      <c r="EN38" s="7"/>
+      <c r="EO38" s="7"/>
+      <c r="EP38" s="7"/>
+      <c r="EQ38" s="7"/>
+      <c r="ER38" s="7"/>
+      <c r="ES38" s="7"/>
+      <c r="ET38" s="7"/>
+      <c r="EU38" s="7"/>
+      <c r="EV38" s="7"/>
+      <c r="EW38" s="7"/>
+      <c r="EX38" s="7"/>
+      <c r="EY38" s="7"/>
+      <c r="EZ38" s="7"/>
+      <c r="FA38" s="7"/>
+      <c r="FB38" s="7"/>
+      <c r="FC38" s="7"/>
+      <c r="FD38" s="7"/>
+      <c r="FE38" s="7"/>
+      <c r="FF38" s="7"/>
+      <c r="FG38" s="7"/>
+      <c r="FH38" s="7"/>
+      <c r="FI38" s="7"/>
+      <c r="FJ38" s="7"/>
+      <c r="FK38" s="7"/>
+      <c r="FL38" s="7"/>
+      <c r="FM38" s="7"/>
+      <c r="FN38" s="7"/>
+      <c r="FO38" s="7"/>
+      <c r="FP38" s="7"/>
+      <c r="FQ38" s="7"/>
+      <c r="FR38" s="7"/>
+      <c r="FS38" s="7"/>
+      <c r="FT38" s="7"/>
+      <c r="FU38" s="7"/>
+      <c r="FV38" s="7"/>
+      <c r="FW38" s="7"/>
+      <c r="FX38" s="7"/>
+      <c r="FY38" s="7"/>
+      <c r="FZ38" s="7"/>
+      <c r="GA38" s="7"/>
+      <c r="GB38" s="7"/>
+      <c r="GC38" s="7"/>
+      <c r="GD38" s="7"/>
+      <c r="GE38" s="7"/>
+      <c r="GF38" s="7"/>
+      <c r="GG38" s="7"/>
+      <c r="GH38" s="7"/>
+      <c r="GI38" s="7"/>
+      <c r="GJ38" s="7"/>
+      <c r="GK38" s="7"/>
+      <c r="GL38" s="7"/>
+      <c r="GM38" s="7"/>
+      <c r="GN38" s="7"/>
+      <c r="GO38" s="7"/>
+      <c r="GP38" s="7"/>
+      <c r="GQ38" s="7"/>
+      <c r="GR38" s="7"/>
+      <c r="GS38" s="7"/>
+      <c r="GT38" s="7"/>
+      <c r="GU38" s="7"/>
+      <c r="GV38" s="7"/>
+      <c r="GW38" s="7"/>
+      <c r="GX38" s="7"/>
+      <c r="GY38" s="7"/>
+      <c r="GZ38" s="7"/>
+      <c r="HA38" s="7"/>
+      <c r="HB38" s="7"/>
+      <c r="HC38" s="7"/>
+      <c r="HD38" s="7"/>
+      <c r="HE38" s="7"/>
+      <c r="HF38" s="7"/>
+      <c r="HG38" s="7"/>
+      <c r="HH38" s="7"/>
+      <c r="HI38" s="7"/>
+      <c r="HJ38" s="7"/>
+      <c r="HK38" s="7"/>
+      <c r="HL38" s="7"/>
+      <c r="HM38" s="7"/>
+      <c r="HN38" s="7"/>
+      <c r="HO38" s="7"/>
+      <c r="HP38" s="7"/>
+      <c r="HQ38" s="7"/>
+      <c r="HR38" s="7"/>
+      <c r="HS38" s="7"/>
+      <c r="HT38" s="7"/>
+      <c r="HU38" s="7"/>
+      <c r="HV38" s="7"/>
+      <c r="HW38" s="7"/>
+      <c r="HX38" s="7"/>
+      <c r="HY38" s="7"/>
+      <c r="HZ38" s="7"/>
+      <c r="IA38" s="7"/>
+      <c r="IB38" s="7"/>
+      <c r="IC38" s="7"/>
+      <c r="ID38" s="7"/>
+      <c r="IE38" s="7"/>
+      <c r="IF38" s="7"/>
+      <c r="IG38" s="7"/>
+      <c r="IH38" s="7"/>
+      <c r="II38" s="7"/>
+      <c r="IJ38" s="7"/>
+      <c r="IK38" s="7"/>
+      <c r="IL38" s="7"/>
+      <c r="IM38" s="7"/>
+      <c r="IN38" s="7"/>
+      <c r="IO38" s="7"/>
+      <c r="IP38" s="7"/>
+      <c r="IQ38" s="7"/>
+      <c r="IR38" s="7"/>
+      <c r="IS38" s="7"/>
+      <c r="IT38" s="7"/>
+      <c r="IU38" s="7"/>
+      <c r="IV38" s="7"/>
+      <c r="IW38" s="7"/>
+      <c r="IX38" s="7"/>
+      <c r="IY38" s="7"/>
+      <c r="IZ38" s="7"/>
+      <c r="JA38" s="7"/>
+      <c r="JB38" s="7"/>
+      <c r="JC38" s="7"/>
+      <c r="JD38" s="7"/>
+      <c r="JE38" s="7"/>
+      <c r="JF38" s="7"/>
+      <c r="JG38" s="7"/>
+      <c r="JH38" s="7"/>
+      <c r="JI38" s="7"/>
+      <c r="JJ38" s="7"/>
+      <c r="JK38" s="7"/>
+      <c r="JL38" s="7"/>
+      <c r="JM38" s="7"/>
+      <c r="JN38" s="7"/>
+      <c r="JO38" s="7"/>
+      <c r="JP38" s="7"/>
+      <c r="JQ38" s="7"/>
+      <c r="JR38" s="7"/>
+      <c r="JS38" s="7"/>
+      <c r="JT38" s="7"/>
+      <c r="JU38" s="7"/>
+      <c r="JV38" s="7"/>
+      <c r="JW38" s="7"/>
+      <c r="JX38" s="7"/>
+      <c r="JY38" s="7"/>
+      <c r="JZ38" s="7"/>
+      <c r="KA38" s="7"/>
+      <c r="KB38" s="7"/>
+      <c r="KC38" s="7"/>
+      <c r="KD38" s="7"/>
+      <c r="KE38" s="7"/>
+      <c r="KF38" s="7"/>
+      <c r="KG38" s="7"/>
+      <c r="KH38" s="7"/>
+      <c r="KI38" s="7"/>
+      <c r="KJ38" s="7"/>
+      <c r="KK38" s="7"/>
+      <c r="KL38" s="7"/>
+      <c r="KM38" s="7"/>
+      <c r="KN38" s="7"/>
+      <c r="KO38" s="7"/>
+      <c r="KP38" s="7"/>
+      <c r="KQ38" s="7"/>
+      <c r="KR38" s="7"/>
+      <c r="KS38" s="7"/>
+      <c r="KT38" s="7"/>
+      <c r="KU38" s="7"/>
+      <c r="KV38" s="7"/>
+      <c r="KW38" s="7"/>
+      <c r="KX38" s="7"/>
+      <c r="KY38" s="7"/>
+      <c r="KZ38" s="7"/>
+      <c r="LA38" s="7"/>
+      <c r="LB38" s="7"/>
+      <c r="LC38" s="7"/>
+      <c r="LD38" s="7"/>
+      <c r="LE38" s="7"/>
+      <c r="LF38" s="7"/>
+      <c r="LG38" s="7"/>
+      <c r="LH38" s="7"/>
+      <c r="LI38" s="7"/>
+      <c r="LJ38" s="7"/>
+      <c r="LK38" s="7"/>
+      <c r="LL38" s="7"/>
+      <c r="LM38" s="7"/>
+      <c r="LN38" s="7"/>
+      <c r="LO38" s="7"/>
+      <c r="LP38" s="7"/>
+      <c r="LQ38" s="7"/>
+      <c r="LR38" s="7"/>
+      <c r="LS38" s="7"/>
+      <c r="LT38" s="7"/>
+      <c r="LU38" s="7"/>
+      <c r="LV38" s="7"/>
+      <c r="LW38" s="7"/>
+      <c r="LX38" s="7"/>
+      <c r="LY38" s="7"/>
+      <c r="LZ38" s="7"/>
+      <c r="MA38" s="7"/>
+      <c r="MB38" s="7"/>
+      <c r="MC38" s="7"/>
+      <c r="MD38" s="7"/>
+      <c r="ME38" s="7"/>
+      <c r="MF38" s="7"/>
+      <c r="MG38" s="7"/>
+      <c r="MH38" s="7"/>
+      <c r="MI38" s="7"/>
+      <c r="MJ38" s="7"/>
+      <c r="MK38" s="7"/>
+      <c r="ML38" s="7"/>
+      <c r="MM38" s="7"/>
+      <c r="MN38" s="7"/>
+      <c r="MO38" s="7"/>
+      <c r="MP38" s="7"/>
+      <c r="MQ38" s="7"/>
+      <c r="MR38" s="7"/>
+      <c r="MS38" s="7"/>
+      <c r="MT38" s="7"/>
+      <c r="MU38" s="7"/>
+      <c r="MV38" s="7"/>
+      <c r="MW38" s="7"/>
+      <c r="MX38" s="7"/>
+      <c r="MY38" s="7"/>
+      <c r="MZ38" s="7"/>
+      <c r="NA38" s="7"/>
+      <c r="NB38" s="7"/>
+      <c r="NC38" s="7"/>
+      <c r="ND38" s="7"/>
+      <c r="NE38" s="7"/>
+      <c r="NF38" s="7"/>
+      <c r="NG38" s="7"/>
+      <c r="NH38" s="7"/>
+      <c r="NI38" s="7"/>
+      <c r="NJ38" s="7"/>
+      <c r="NK38" s="7"/>
+      <c r="NL38" s="7"/>
+      <c r="NM38" s="7"/>
+      <c r="NN38" s="7"/>
+      <c r="NO38" s="7"/>
+      <c r="NP38" s="7"/>
+      <c r="NQ38" s="7"/>
+      <c r="NR38" s="7"/>
+      <c r="NS38" s="7"/>
+      <c r="NT38" s="7"/>
+      <c r="NU38" s="7"/>
+      <c r="NV38" s="7"/>
+      <c r="NW38" s="7"/>
+      <c r="NX38" s="7"/>
+      <c r="NY38" s="7"/>
+      <c r="NZ38" s="7"/>
+      <c r="OA38" s="7"/>
+      <c r="OB38" s="7"/>
+      <c r="OC38" s="7"/>
+      <c r="OD38" s="7"/>
+      <c r="OE38" s="7"/>
+      <c r="OF38" s="7"/>
+      <c r="OG38" s="7"/>
+      <c r="OH38" s="7"/>
+      <c r="OI38" s="7"/>
+      <c r="OJ38" s="7"/>
+      <c r="OK38" s="7"/>
+      <c r="OL38" s="7"/>
+      <c r="OM38" s="7"/>
+      <c r="ON38" s="7"/>
+      <c r="OO38" s="7"/>
+      <c r="OP38" s="7"/>
+      <c r="OQ38" s="7"/>
+      <c r="OR38" s="7"/>
+      <c r="OS38" s="7"/>
+      <c r="OT38" s="7"/>
+      <c r="OU38" s="7"/>
+      <c r="OV38" s="7"/>
+      <c r="OW38" s="7"/>
+      <c r="OX38" s="7"/>
+      <c r="OY38" s="7"/>
+      <c r="OZ38" s="7"/>
+      <c r="PA38" s="7"/>
+      <c r="PB38" s="7"/>
+      <c r="PC38" s="7"/>
+      <c r="PD38" s="7"/>
+      <c r="PE38" s="7"/>
+      <c r="PF38" s="7"/>
+      <c r="PG38" s="7"/>
+      <c r="PH38" s="7"/>
+      <c r="PI38" s="7"/>
+      <c r="PJ38" s="7"/>
+      <c r="PK38" s="7"/>
+      <c r="PL38" s="7"/>
+      <c r="PM38" s="7"/>
+      <c r="PN38" s="7"/>
+      <c r="PO38" s="7"/>
+      <c r="PP38" s="7"/>
+      <c r="PQ38" s="7"/>
+      <c r="PR38" s="7"/>
+      <c r="PS38" s="7"/>
+      <c r="PT38" s="7"/>
+      <c r="PU38" s="7"/>
+      <c r="PV38" s="7"/>
+      <c r="PW38" s="7"/>
+      <c r="PX38" s="7"/>
+      <c r="PY38" s="7"/>
+      <c r="PZ38" s="7"/>
+      <c r="QA38" s="7"/>
+      <c r="QB38" s="7"/>
+      <c r="QC38" s="7"/>
+      <c r="QD38" s="7"/>
+      <c r="QE38" s="7"/>
+      <c r="QF38" s="7"/>
+      <c r="QG38" s="7"/>
+      <c r="QH38" s="7"/>
+      <c r="QI38" s="7"/>
+      <c r="QJ38" s="7"/>
+      <c r="QK38" s="7"/>
+      <c r="QL38" s="7"/>
+      <c r="QM38" s="7"/>
+      <c r="QN38" s="7"/>
+      <c r="QO38" s="7"/>
+      <c r="QP38" s="7"/>
+      <c r="QQ38" s="7"/>
+      <c r="QR38" s="7"/>
+      <c r="QS38" s="7"/>
+      <c r="QT38" s="7"/>
+      <c r="QU38" s="7"/>
+      <c r="QV38" s="7"/>
+      <c r="QW38" s="7"/>
+      <c r="QX38" s="7"/>
+      <c r="QY38" s="7"/>
+      <c r="QZ38" s="7"/>
+      <c r="RA38" s="7"/>
+      <c r="RB38" s="7"/>
+      <c r="RC38" s="7"/>
+      <c r="RD38" s="7"/>
+      <c r="RE38" s="7"/>
+      <c r="RF38" s="7"/>
+      <c r="RG38" s="7"/>
+      <c r="RH38" s="7"/>
+      <c r="RI38" s="7"/>
+      <c r="RJ38" s="7"/>
+      <c r="RK38" s="7"/>
+      <c r="RL38" s="7"/>
+      <c r="RM38" s="7"/>
+      <c r="RN38" s="7"/>
+      <c r="RO38" s="7"/>
+      <c r="RP38" s="7"/>
+      <c r="RQ38" s="7"/>
+      <c r="RR38" s="7"/>
+      <c r="RS38" s="7"/>
+      <c r="RT38" s="7"/>
+      <c r="RU38" s="7"/>
+      <c r="RV38" s="7"/>
+      <c r="RW38" s="7"/>
+      <c r="RX38" s="7"/>
+      <c r="RY38" s="7"/>
+      <c r="RZ38" s="7"/>
+      <c r="SA38" s="7"/>
+      <c r="SB38" s="7"/>
+      <c r="SC38" s="7"/>
+      <c r="SD38" s="7"/>
+      <c r="SE38" s="7"/>
+      <c r="SF38" s="7"/>
+      <c r="SG38" s="7"/>
+      <c r="SH38" s="7"/>
+      <c r="SI38" s="7"/>
+      <c r="SJ38" s="7"/>
+      <c r="SK38" s="7"/>
+      <c r="SL38" s="7"/>
+      <c r="SM38" s="7"/>
+      <c r="SN38" s="7"/>
+      <c r="SO38" s="7"/>
+      <c r="SP38" s="7"/>
+      <c r="SQ38" s="7"/>
+      <c r="SR38" s="7"/>
+      <c r="SS38" s="7"/>
+      <c r="ST38" s="7"/>
+      <c r="SU38" s="7"/>
+      <c r="SV38" s="7"/>
+      <c r="SW38" s="7"/>
+      <c r="SX38" s="7"/>
+      <c r="SY38" s="7"/>
+      <c r="SZ38" s="7"/>
+      <c r="TA38" s="7"/>
+      <c r="TB38" s="7"/>
+      <c r="TC38" s="7"/>
+      <c r="TD38" s="7"/>
+      <c r="TE38" s="7"/>
+      <c r="TF38" s="7"/>
+      <c r="TG38" s="7"/>
+      <c r="TH38" s="7"/>
+      <c r="TI38" s="7"/>
+      <c r="TJ38" s="7"/>
+      <c r="TK38" s="7"/>
+      <c r="TL38" s="7"/>
+      <c r="TM38" s="7"/>
+      <c r="TN38" s="7"/>
+      <c r="TO38" s="7"/>
+      <c r="TP38" s="7"/>
+      <c r="TQ38" s="7"/>
+      <c r="TR38" s="7"/>
+      <c r="TS38" s="7"/>
+      <c r="TT38" s="7"/>
+      <c r="TU38" s="7"/>
+      <c r="TV38" s="7"/>
+      <c r="TW38" s="7"/>
+      <c r="TX38" s="7"/>
+      <c r="TY38" s="7"/>
+      <c r="TZ38" s="7"/>
+      <c r="UA38" s="7"/>
+      <c r="UB38" s="7"/>
+      <c r="UC38" s="7"/>
+      <c r="UD38" s="7"/>
+      <c r="UE38" s="7"/>
+      <c r="UF38" s="7"/>
+      <c r="UG38" s="7"/>
+      <c r="UH38" s="7"/>
+      <c r="UI38" s="7"/>
+      <c r="UJ38" s="7"/>
+      <c r="UK38" s="7"/>
+      <c r="UL38" s="7"/>
+      <c r="UM38" s="7"/>
+      <c r="UN38" s="7"/>
+      <c r="UO38" s="7"/>
+      <c r="UP38" s="7"/>
+      <c r="UQ38" s="7"/>
+      <c r="UR38" s="7"/>
+      <c r="US38" s="7"/>
+      <c r="UT38" s="7"/>
+      <c r="UU38" s="7"/>
+      <c r="UV38" s="7"/>
+      <c r="UW38" s="7"/>
+      <c r="UX38" s="7"/>
+      <c r="UY38" s="7"/>
+      <c r="UZ38" s="7"/>
+      <c r="VA38" s="7"/>
+      <c r="VB38" s="7"/>
+      <c r="VC38" s="7"/>
+      <c r="VD38" s="7"/>
+      <c r="VE38" s="7"/>
+      <c r="VF38" s="7"/>
+      <c r="VG38" s="7"/>
+      <c r="VH38" s="7"/>
+      <c r="VI38" s="7"/>
+      <c r="VJ38" s="7"/>
+      <c r="VK38" s="7"/>
+      <c r="VL38" s="7"/>
+      <c r="VM38" s="7"/>
+      <c r="VN38" s="7"/>
+      <c r="VO38" s="7"/>
+      <c r="VP38" s="7"/>
+      <c r="VQ38" s="7"/>
+      <c r="VR38" s="7"/>
+      <c r="VS38" s="7"/>
+      <c r="VT38" s="7"/>
+      <c r="VU38" s="7"/>
+      <c r="VV38" s="7"/>
+      <c r="VW38" s="7"/>
+      <c r="VX38" s="7"/>
+      <c r="VY38" s="7"/>
+      <c r="VZ38" s="7"/>
+      <c r="WA38" s="7"/>
+      <c r="WB38" s="7"/>
+      <c r="WC38" s="7"/>
+      <c r="WD38" s="7"/>
+      <c r="WE38" s="7"/>
+      <c r="WF38" s="7"/>
+      <c r="WG38" s="7"/>
+      <c r="WH38" s="7"/>
+      <c r="WI38" s="7"/>
+      <c r="WJ38" s="7"/>
+      <c r="WK38" s="7"/>
+      <c r="WL38" s="7"/>
+      <c r="WM38" s="7"/>
+      <c r="WN38" s="7"/>
+      <c r="WO38" s="7"/>
+      <c r="WP38" s="7"/>
+      <c r="WQ38" s="7"/>
+      <c r="WR38" s="7"/>
+      <c r="WS38" s="7"/>
+      <c r="WT38" s="7"/>
+      <c r="WU38" s="7"/>
+      <c r="WV38" s="7"/>
+      <c r="WW38" s="7"/>
+      <c r="WX38" s="7"/>
+      <c r="WY38" s="7"/>
+      <c r="WZ38" s="7"/>
+      <c r="XA38" s="7"/>
+      <c r="XB38" s="7"/>
+      <c r="XC38" s="7"/>
+      <c r="XD38" s="7"/>
+      <c r="XE38" s="7"/>
+      <c r="XF38" s="7"/>
+      <c r="XG38" s="7"/>
+      <c r="XH38" s="7"/>
+      <c r="XI38" s="7"/>
+      <c r="XJ38" s="7"/>
+      <c r="XK38" s="7"/>
+      <c r="XL38" s="7"/>
+      <c r="XM38" s="7"/>
+      <c r="XN38" s="7"/>
+      <c r="XO38" s="7"/>
+      <c r="XP38" s="7"/>
+      <c r="XQ38" s="7"/>
+      <c r="XR38" s="7"/>
+      <c r="XS38" s="7"/>
+      <c r="XT38" s="7"/>
+      <c r="XU38" s="7"/>
+      <c r="XV38" s="7"/>
+      <c r="XW38" s="7"/>
+      <c r="XX38" s="7"/>
+      <c r="XY38" s="7"/>
+      <c r="XZ38" s="7"/>
+      <c r="YA38" s="7"/>
+      <c r="YB38" s="7"/>
+      <c r="YC38" s="7"/>
+      <c r="YD38" s="7"/>
+      <c r="YE38" s="7"/>
+      <c r="YF38" s="7"/>
+      <c r="YG38" s="7"/>
+      <c r="YH38" s="7"/>
+      <c r="YI38" s="7"/>
+      <c r="YJ38" s="7"/>
+      <c r="YK38" s="7"/>
+      <c r="YL38" s="7"/>
+      <c r="YM38" s="7"/>
+      <c r="YN38" s="7"/>
+      <c r="YO38" s="7"/>
+      <c r="YP38" s="7"/>
+      <c r="YQ38" s="7"/>
+      <c r="YR38" s="7"/>
+      <c r="YS38" s="7"/>
+      <c r="YT38" s="7"/>
+      <c r="YU38" s="7"/>
+      <c r="YV38" s="7"/>
+      <c r="YW38" s="7"/>
+      <c r="YX38" s="7"/>
+      <c r="YY38" s="7"/>
+      <c r="YZ38" s="7"/>
+      <c r="ZA38" s="7"/>
+      <c r="ZB38" s="7"/>
+      <c r="ZC38" s="7"/>
+      <c r="ZD38" s="7"/>
+      <c r="ZE38" s="7"/>
+      <c r="ZF38" s="7"/>
+      <c r="ZG38" s="7"/>
+      <c r="ZH38" s="7"/>
+      <c r="ZI38" s="7"/>
+      <c r="ZJ38" s="7"/>
+      <c r="ZK38" s="7"/>
+      <c r="ZL38" s="7"/>
+      <c r="ZM38" s="7"/>
+      <c r="ZN38" s="7"/>
+      <c r="ZO38" s="7"/>
+      <c r="ZP38" s="7"/>
+      <c r="ZQ38" s="7"/>
+      <c r="ZR38" s="7"/>
+      <c r="ZS38" s="7"/>
+      <c r="ZT38" s="7"/>
+      <c r="ZU38" s="7"/>
+      <c r="ZV38" s="7"/>
+      <c r="ZW38" s="7"/>
+      <c r="ZX38" s="7"/>
+      <c r="ZY38" s="7"/>
+      <c r="ZZ38" s="7"/>
+      <c r="AAA38" s="7"/>
+      <c r="AAB38" s="7"/>
+      <c r="AAC38" s="7"/>
+      <c r="AAD38" s="7"/>
+      <c r="AAE38" s="7"/>
+      <c r="AAF38" s="7"/>
+      <c r="AAG38" s="7"/>
+      <c r="AAH38" s="7"/>
+      <c r="AAI38" s="7"/>
+      <c r="AAJ38" s="7"/>
+      <c r="AAK38" s="7"/>
+      <c r="AAL38" s="7"/>
+      <c r="AAM38" s="7"/>
+      <c r="AAN38" s="7"/>
+      <c r="AAO38" s="7"/>
+      <c r="AAP38" s="7"/>
+      <c r="AAQ38" s="7"/>
+      <c r="AAR38" s="7"/>
+      <c r="AAS38" s="7"/>
+      <c r="AAT38" s="7"/>
+      <c r="AAU38" s="7"/>
+      <c r="AAV38" s="7"/>
+      <c r="AAW38" s="7"/>
+      <c r="AAX38" s="7"/>
+      <c r="AAY38" s="7"/>
+      <c r="AAZ38" s="7"/>
+      <c r="ABA38" s="7"/>
+      <c r="ABB38" s="7"/>
+      <c r="ABC38" s="7"/>
+      <c r="ABD38" s="7"/>
+      <c r="ABE38" s="7"/>
+      <c r="ABF38" s="7"/>
+      <c r="ABG38" s="7"/>
+      <c r="ABH38" s="7"/>
+      <c r="ABI38" s="7"/>
+      <c r="ABJ38" s="7"/>
+      <c r="ABK38" s="7"/>
+      <c r="ABL38" s="7"/>
+      <c r="ABM38" s="7"/>
+      <c r="ABN38" s="7"/>
+      <c r="ABO38" s="7"/>
+      <c r="ABP38" s="7"/>
+      <c r="ABQ38" s="7"/>
+      <c r="ABR38" s="7"/>
+      <c r="ABS38" s="7"/>
+      <c r="ABT38" s="7"/>
+      <c r="ABU38" s="7"/>
+      <c r="ABV38" s="7"/>
+      <c r="ABW38" s="7"/>
+      <c r="ABX38" s="7"/>
+      <c r="ABY38" s="7"/>
+      <c r="ABZ38" s="7"/>
+      <c r="ACA38" s="7"/>
+      <c r="ACB38" s="7"/>
+      <c r="ACC38" s="7"/>
+      <c r="ACD38" s="7"/>
+      <c r="ACE38" s="7"/>
+      <c r="ACF38" s="7"/>
+      <c r="ACG38" s="7"/>
+      <c r="ACH38" s="7"/>
+      <c r="ACI38" s="7"/>
+      <c r="ACJ38" s="7"/>
+      <c r="ACK38" s="7"/>
+      <c r="ACL38" s="7"/>
+      <c r="ACM38" s="7"/>
+      <c r="ACN38" s="7"/>
+      <c r="ACO38" s="7"/>
+      <c r="ACP38" s="7"/>
+      <c r="ACQ38" s="7"/>
+      <c r="ACR38" s="7"/>
+      <c r="ACS38" s="7"/>
+      <c r="ACT38" s="7"/>
+      <c r="ACU38" s="7"/>
+      <c r="ACV38" s="7"/>
+      <c r="ACW38" s="7"/>
+      <c r="ACX38" s="7"/>
+      <c r="ACY38" s="7"/>
+      <c r="ACZ38" s="7"/>
+      <c r="ADA38" s="7"/>
+      <c r="ADB38" s="7"/>
+      <c r="ADC38" s="7"/>
+      <c r="ADD38" s="7"/>
+      <c r="ADE38" s="7"/>
+      <c r="ADF38" s="7"/>
+      <c r="ADG38" s="7"/>
+      <c r="ADH38" s="7"/>
+      <c r="ADI38" s="7"/>
+      <c r="ADJ38" s="7"/>
+      <c r="ADK38" s="7"/>
+      <c r="ADL38" s="7"/>
+      <c r="ADM38" s="7"/>
+      <c r="ADN38" s="7"/>
+      <c r="ADO38" s="7"/>
+      <c r="ADP38" s="7"/>
+      <c r="ADQ38" s="7"/>
+      <c r="ADR38" s="7"/>
+      <c r="ADS38" s="7"/>
+      <c r="ADT38" s="7"/>
+      <c r="ADU38" s="7"/>
+      <c r="ADV38" s="7"/>
+      <c r="ADW38" s="7"/>
+      <c r="ADX38" s="7"/>
+      <c r="ADY38" s="7"/>
+      <c r="ADZ38" s="7"/>
+      <c r="AEA38" s="7"/>
+      <c r="AEB38" s="7"/>
+      <c r="AEC38" s="7"/>
+      <c r="AED38" s="7"/>
+      <c r="AEE38" s="7"/>
+      <c r="AEF38" s="7"/>
+      <c r="AEG38" s="7"/>
+      <c r="AEH38" s="7"/>
+      <c r="AEI38" s="7"/>
+      <c r="AEJ38" s="7"/>
+      <c r="AEK38" s="7"/>
+      <c r="AEL38" s="7"/>
+      <c r="AEM38" s="7"/>
+      <c r="AEN38" s="7"/>
+      <c r="AEO38" s="7"/>
+      <c r="AEP38" s="7"/>
+      <c r="AEQ38" s="7"/>
+      <c r="AER38" s="7"/>
+      <c r="AES38" s="7"/>
+      <c r="AET38" s="7"/>
+      <c r="AEU38" s="7"/>
+      <c r="AEV38" s="7"/>
+      <c r="AEW38" s="7"/>
+      <c r="AEX38" s="7"/>
+      <c r="AEY38" s="7"/>
+      <c r="AEZ38" s="7"/>
+      <c r="AFA38" s="7"/>
+      <c r="AFB38" s="7"/>
+      <c r="AFC38" s="7"/>
+      <c r="AFD38" s="7"/>
+      <c r="AFE38" s="7"/>
+      <c r="AFF38" s="7"/>
+      <c r="AFG38" s="7"/>
+      <c r="AFH38" s="7"/>
+      <c r="AFI38" s="7"/>
+      <c r="AFJ38" s="7"/>
+      <c r="AFK38" s="7"/>
+      <c r="AFL38" s="7"/>
+      <c r="AFM38" s="7"/>
+      <c r="AFN38" s="7"/>
+      <c r="AFO38" s="7"/>
+      <c r="AFP38" s="7"/>
+      <c r="AFQ38" s="7"/>
+      <c r="AFR38" s="7"/>
+      <c r="AFS38" s="7"/>
+      <c r="AFT38" s="7"/>
+      <c r="AFU38" s="7"/>
+      <c r="AFV38" s="7"/>
+      <c r="AFW38" s="7"/>
+      <c r="AFX38" s="7"/>
+      <c r="AFY38" s="7"/>
+      <c r="AFZ38" s="7"/>
+      <c r="AGA38" s="7"/>
+      <c r="AGB38" s="7"/>
+      <c r="AGC38" s="7"/>
+      <c r="AGD38" s="7"/>
+      <c r="AGE38" s="7"/>
+      <c r="AGF38" s="7"/>
+      <c r="AGG38" s="7"/>
+      <c r="AGH38" s="7"/>
+      <c r="AGI38" s="7"/>
+      <c r="AGJ38" s="7"/>
+      <c r="AGK38" s="7"/>
+      <c r="AGL38" s="7"/>
+      <c r="AGM38" s="7"/>
+      <c r="AGN38" s="7"/>
+      <c r="AGO38" s="7"/>
+      <c r="AGP38" s="7"/>
+      <c r="AGQ38" s="7"/>
+      <c r="AGR38" s="7"/>
+      <c r="AGS38" s="7"/>
+      <c r="AGT38" s="7"/>
+      <c r="AGU38" s="7"/>
+      <c r="AGV38" s="7"/>
+      <c r="AGW38" s="7"/>
+      <c r="AGX38" s="7"/>
+      <c r="AGY38" s="7"/>
+      <c r="AGZ38" s="7"/>
+      <c r="AHA38" s="7"/>
+      <c r="AHB38" s="7"/>
+      <c r="AHC38" s="7"/>
+      <c r="AHD38" s="7"/>
+      <c r="AHE38" s="7"/>
+      <c r="AHF38" s="7"/>
+      <c r="AHG38" s="7"/>
+      <c r="AHH38" s="7"/>
+      <c r="AHI38" s="7"/>
+      <c r="AHJ38" s="7"/>
+      <c r="AHK38" s="7"/>
+      <c r="AHL38" s="7"/>
+      <c r="AHM38" s="7"/>
+      <c r="AHN38" s="7"/>
+      <c r="AHO38" s="7"/>
+      <c r="AHP38" s="7"/>
+      <c r="AHQ38" s="7"/>
+      <c r="AHR38" s="7"/>
+      <c r="AHS38" s="7"/>
+      <c r="AHT38" s="7"/>
+      <c r="AHU38" s="7"/>
+      <c r="AHV38" s="7"/>
+      <c r="AHW38" s="7"/>
+      <c r="AHX38" s="7"/>
+      <c r="AHY38" s="7"/>
+      <c r="AHZ38" s="7"/>
+      <c r="AIA38" s="7"/>
+      <c r="AIB38" s="7"/>
+      <c r="AIC38" s="7"/>
+      <c r="AID38" s="7"/>
+      <c r="AIE38" s="7"/>
+      <c r="AIF38" s="7"/>
+      <c r="AIG38" s="7"/>
+      <c r="AIH38" s="7"/>
+      <c r="AII38" s="7"/>
+      <c r="AIJ38" s="7"/>
+      <c r="AIK38" s="7"/>
+      <c r="AIL38" s="7"/>
+      <c r="AIM38" s="7"/>
+      <c r="AIN38" s="7"/>
+      <c r="AIO38" s="7"/>
+      <c r="AIP38" s="7"/>
+      <c r="AIQ38" s="7"/>
+      <c r="AIR38" s="7"/>
+      <c r="AIS38" s="7"/>
+      <c r="AIT38" s="7"/>
+      <c r="AIU38" s="7"/>
+      <c r="AIV38" s="7"/>
+      <c r="AIW38" s="7"/>
+      <c r="AIX38" s="7"/>
+      <c r="AIY38" s="7"/>
+      <c r="AIZ38" s="7"/>
+      <c r="AJA38" s="7"/>
+      <c r="AJB38" s="7"/>
+      <c r="AJC38" s="7"/>
+      <c r="AJD38" s="7"/>
+      <c r="AJE38" s="7"/>
+      <c r="AJF38" s="7"/>
+      <c r="AJG38" s="7"/>
+      <c r="AJH38" s="7"/>
+      <c r="AJI38" s="7"/>
+      <c r="AJJ38" s="7"/>
+      <c r="AJK38" s="7"/>
+      <c r="AJL38" s="7"/>
+      <c r="AJM38" s="7"/>
+      <c r="AJN38" s="7"/>
+      <c r="AJO38" s="7"/>
+      <c r="AJP38" s="7"/>
+      <c r="AJQ38" s="7"/>
+      <c r="AJR38" s="7"/>
+      <c r="AJS38" s="7"/>
+      <c r="AJT38" s="7"/>
+      <c r="AJU38" s="7"/>
+      <c r="AJV38" s="7"/>
+      <c r="AJW38" s="7"/>
+      <c r="AJX38" s="7"/>
+      <c r="AJY38" s="7"/>
+      <c r="AJZ38" s="7"/>
+      <c r="AKA38" s="7"/>
+      <c r="AKB38" s="7"/>
+      <c r="AKC38" s="7"/>
+      <c r="AKD38" s="7"/>
+      <c r="AKE38" s="7"/>
+      <c r="AKF38" s="7"/>
+      <c r="AKG38" s="7"/>
+      <c r="AKH38" s="7"/>
+      <c r="AKI38" s="7"/>
+      <c r="AKJ38" s="7"/>
+      <c r="AKK38" s="7"/>
+      <c r="AKL38" s="7"/>
+      <c r="AKM38" s="7"/>
+      <c r="AKN38" s="7"/>
+      <c r="AKO38" s="7"/>
+      <c r="AKP38" s="7"/>
+      <c r="AKQ38" s="7"/>
+      <c r="AKR38" s="7"/>
+      <c r="AKS38" s="7"/>
+      <c r="AKT38" s="7"/>
+      <c r="AKU38" s="7"/>
+      <c r="AKV38" s="7"/>
+      <c r="AKW38" s="7"/>
+      <c r="AKX38" s="7"/>
+      <c r="AKY38" s="7"/>
+      <c r="AKZ38" s="7"/>
+      <c r="ALA38" s="7"/>
+      <c r="ALB38" s="7"/>
+      <c r="ALC38" s="7"/>
+      <c r="ALD38" s="7"/>
+      <c r="ALE38" s="7"/>
+      <c r="ALF38" s="7"/>
+      <c r="ALG38" s="7"/>
+      <c r="ALH38" s="7"/>
+      <c r="ALI38" s="7"/>
+      <c r="ALJ38" s="7"/>
+      <c r="ALK38" s="7"/>
+      <c r="ALL38" s="7"/>
+      <c r="ALM38" s="7"/>
+      <c r="ALN38" s="7"/>
+      <c r="ALO38" s="7"/>
+      <c r="ALP38" s="7"/>
+      <c r="ALQ38" s="7"/>
+      <c r="ALR38" s="7"/>
+      <c r="ALS38" s="7"/>
+      <c r="ALT38" s="7"/>
+      <c r="ALU38" s="7"/>
+      <c r="ALV38" s="7"/>
+      <c r="ALW38" s="7"/>
+      <c r="ALX38" s="7"/>
+      <c r="ALY38" s="7"/>
+      <c r="ALZ38" s="7"/>
+      <c r="AMA38" s="7"/>
+      <c r="AMB38" s="7"/>
+      <c r="AMC38" s="7"/>
+      <c r="AMD38" s="7"/>
+      <c r="AME38" s="7"/>
+      <c r="AMF38" s="7"/>
+      <c r="AMG38" s="7"/>
+      <c r="AMH38" s="7"/>
+      <c r="AMI38" s="7"/>
+      <c r="AMJ38" s="7"/>
+      <c r="AMK38" s="7"/>
+    </row>
+    <row r="39" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="4" t="s">
+    </row>
+    <row r="40" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="4" t="s">
+    </row>
+    <row r="41" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="B42" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
+      <c r="C42" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="1" t="s">
+    </row>
+    <row r="43" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A43" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="B43" s="7" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
+      <c r="C43" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="1" t="s">
+    </row>
+    <row r="44" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="B44" s="7" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
+      <c r="C44" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="1" t="s">
+    </row>
+    <row r="45" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="B45" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
+      <c r="C45" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B45" s="1" t="s">
+    </row>
+    <row r="46" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="B46" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
+      <c r="C46" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B46" s="1" t="s">
+    </row>
+    <row r="47" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="B47" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
+      <c r="C47" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="B48" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
+      <c r="C48" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="5" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="5" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C50" s="9" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
+      <c r="B51" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="4" t="s">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="6" t="s">
+      <c r="B52" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>155</v>
       </c>
@@ -1867,18 +2963,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>161</v>
       </c>
@@ -1889,7 +2985,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>164</v>
       </c>
@@ -1900,7 +2996,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>167</v>
       </c>
@@ -1911,7 +3007,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -1922,238 +3018,1364 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C61" s="4" t="s">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C62" s="4" t="s">
+    </row>
+    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C63" s="5" t="s">
+    </row>
+    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C64" s="4" t="s">
+    </row>
+    <row r="65" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
+      <c r="B65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B65" s="1" t="s">
+    </row>
+    <row r="66" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A66" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="B66" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C67" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C68" s="11" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C70" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C73" s="9" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="7" t="s">
+    <row r="74" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B74" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C74" s="10" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="7" t="s">
+    <row r="75" spans="1:1025" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B75" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C75" s="11" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" s="7" customFormat="1" ht="15">
-      <c r="A75" s="8" t="s">
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+      <c r="AE75" s="1"/>
+      <c r="AF75" s="1"/>
+      <c r="AG75" s="1"/>
+      <c r="AH75" s="1"/>
+      <c r="AI75" s="1"/>
+      <c r="AJ75" s="1"/>
+      <c r="AK75" s="1"/>
+      <c r="AL75" s="1"/>
+      <c r="AM75" s="1"/>
+      <c r="AN75" s="1"/>
+      <c r="AO75" s="1"/>
+      <c r="AP75" s="1"/>
+      <c r="AQ75" s="1"/>
+      <c r="AR75" s="1"/>
+      <c r="AS75" s="1"/>
+      <c r="AT75" s="1"/>
+      <c r="AU75" s="1"/>
+      <c r="AV75" s="1"/>
+      <c r="AW75" s="1"/>
+      <c r="AX75" s="1"/>
+      <c r="AY75" s="1"/>
+      <c r="AZ75" s="1"/>
+      <c r="BA75" s="1"/>
+      <c r="BB75" s="1"/>
+      <c r="BC75" s="1"/>
+      <c r="BD75" s="1"/>
+      <c r="BE75" s="1"/>
+      <c r="BF75" s="1"/>
+      <c r="BG75" s="1"/>
+      <c r="BH75" s="1"/>
+      <c r="BI75" s="1"/>
+      <c r="BJ75" s="1"/>
+      <c r="BK75" s="1"/>
+      <c r="BL75" s="1"/>
+      <c r="BM75" s="1"/>
+      <c r="BN75" s="1"/>
+      <c r="BO75" s="1"/>
+      <c r="BP75" s="1"/>
+      <c r="BQ75" s="1"/>
+      <c r="BR75" s="1"/>
+      <c r="BS75" s="1"/>
+      <c r="BT75" s="1"/>
+      <c r="BU75" s="1"/>
+      <c r="BV75" s="1"/>
+      <c r="BW75" s="1"/>
+      <c r="BX75" s="1"/>
+      <c r="BY75" s="1"/>
+      <c r="BZ75" s="1"/>
+      <c r="CA75" s="1"/>
+      <c r="CB75" s="1"/>
+      <c r="CC75" s="1"/>
+      <c r="CD75" s="1"/>
+      <c r="CE75" s="1"/>
+      <c r="CF75" s="1"/>
+      <c r="CG75" s="1"/>
+      <c r="CH75" s="1"/>
+      <c r="CI75" s="1"/>
+      <c r="CJ75" s="1"/>
+      <c r="CK75" s="1"/>
+      <c r="CL75" s="1"/>
+      <c r="CM75" s="1"/>
+      <c r="CN75" s="1"/>
+      <c r="CO75" s="1"/>
+      <c r="CP75" s="1"/>
+      <c r="CQ75" s="1"/>
+      <c r="CR75" s="1"/>
+      <c r="CS75" s="1"/>
+      <c r="CT75" s="1"/>
+      <c r="CU75" s="1"/>
+      <c r="CV75" s="1"/>
+      <c r="CW75" s="1"/>
+      <c r="CX75" s="1"/>
+      <c r="CY75" s="1"/>
+      <c r="CZ75" s="1"/>
+      <c r="DA75" s="1"/>
+      <c r="DB75" s="1"/>
+      <c r="DC75" s="1"/>
+      <c r="DD75" s="1"/>
+      <c r="DE75" s="1"/>
+      <c r="DF75" s="1"/>
+      <c r="DG75" s="1"/>
+      <c r="DH75" s="1"/>
+      <c r="DI75" s="1"/>
+      <c r="DJ75" s="1"/>
+      <c r="DK75" s="1"/>
+      <c r="DL75" s="1"/>
+      <c r="DM75" s="1"/>
+      <c r="DN75" s="1"/>
+      <c r="DO75" s="1"/>
+      <c r="DP75" s="1"/>
+      <c r="DQ75" s="1"/>
+      <c r="DR75" s="1"/>
+      <c r="DS75" s="1"/>
+      <c r="DT75" s="1"/>
+      <c r="DU75" s="1"/>
+      <c r="DV75" s="1"/>
+      <c r="DW75" s="1"/>
+      <c r="DX75" s="1"/>
+      <c r="DY75" s="1"/>
+      <c r="DZ75" s="1"/>
+      <c r="EA75" s="1"/>
+      <c r="EB75" s="1"/>
+      <c r="EC75" s="1"/>
+      <c r="ED75" s="1"/>
+      <c r="EE75" s="1"/>
+      <c r="EF75" s="1"/>
+      <c r="EG75" s="1"/>
+      <c r="EH75" s="1"/>
+      <c r="EI75" s="1"/>
+      <c r="EJ75" s="1"/>
+      <c r="EK75" s="1"/>
+      <c r="EL75" s="1"/>
+      <c r="EM75" s="1"/>
+      <c r="EN75" s="1"/>
+      <c r="EO75" s="1"/>
+      <c r="EP75" s="1"/>
+      <c r="EQ75" s="1"/>
+      <c r="ER75" s="1"/>
+      <c r="ES75" s="1"/>
+      <c r="ET75" s="1"/>
+      <c r="EU75" s="1"/>
+      <c r="EV75" s="1"/>
+      <c r="EW75" s="1"/>
+      <c r="EX75" s="1"/>
+      <c r="EY75" s="1"/>
+      <c r="EZ75" s="1"/>
+      <c r="FA75" s="1"/>
+      <c r="FB75" s="1"/>
+      <c r="FC75" s="1"/>
+      <c r="FD75" s="1"/>
+      <c r="FE75" s="1"/>
+      <c r="FF75" s="1"/>
+      <c r="FG75" s="1"/>
+      <c r="FH75" s="1"/>
+      <c r="FI75" s="1"/>
+      <c r="FJ75" s="1"/>
+      <c r="FK75" s="1"/>
+      <c r="FL75" s="1"/>
+      <c r="FM75" s="1"/>
+      <c r="FN75" s="1"/>
+      <c r="FO75" s="1"/>
+      <c r="FP75" s="1"/>
+      <c r="FQ75" s="1"/>
+      <c r="FR75" s="1"/>
+      <c r="FS75" s="1"/>
+      <c r="FT75" s="1"/>
+      <c r="FU75" s="1"/>
+      <c r="FV75" s="1"/>
+      <c r="FW75" s="1"/>
+      <c r="FX75" s="1"/>
+      <c r="FY75" s="1"/>
+      <c r="FZ75" s="1"/>
+      <c r="GA75" s="1"/>
+      <c r="GB75" s="1"/>
+      <c r="GC75" s="1"/>
+      <c r="GD75" s="1"/>
+      <c r="GE75" s="1"/>
+      <c r="GF75" s="1"/>
+      <c r="GG75" s="1"/>
+      <c r="GH75" s="1"/>
+      <c r="GI75" s="1"/>
+      <c r="GJ75" s="1"/>
+      <c r="GK75" s="1"/>
+      <c r="GL75" s="1"/>
+      <c r="GM75" s="1"/>
+      <c r="GN75" s="1"/>
+      <c r="GO75" s="1"/>
+      <c r="GP75" s="1"/>
+      <c r="GQ75" s="1"/>
+      <c r="GR75" s="1"/>
+      <c r="GS75" s="1"/>
+      <c r="GT75" s="1"/>
+      <c r="GU75" s="1"/>
+      <c r="GV75" s="1"/>
+      <c r="GW75" s="1"/>
+      <c r="GX75" s="1"/>
+      <c r="GY75" s="1"/>
+      <c r="GZ75" s="1"/>
+      <c r="HA75" s="1"/>
+      <c r="HB75" s="1"/>
+      <c r="HC75" s="1"/>
+      <c r="HD75" s="1"/>
+      <c r="HE75" s="1"/>
+      <c r="HF75" s="1"/>
+      <c r="HG75" s="1"/>
+      <c r="HH75" s="1"/>
+      <c r="HI75" s="1"/>
+      <c r="HJ75" s="1"/>
+      <c r="HK75" s="1"/>
+      <c r="HL75" s="1"/>
+      <c r="HM75" s="1"/>
+      <c r="HN75" s="1"/>
+      <c r="HO75" s="1"/>
+      <c r="HP75" s="1"/>
+      <c r="HQ75" s="1"/>
+      <c r="HR75" s="1"/>
+      <c r="HS75" s="1"/>
+      <c r="HT75" s="1"/>
+      <c r="HU75" s="1"/>
+      <c r="HV75" s="1"/>
+      <c r="HW75" s="1"/>
+      <c r="HX75" s="1"/>
+      <c r="HY75" s="1"/>
+      <c r="HZ75" s="1"/>
+      <c r="IA75" s="1"/>
+      <c r="IB75" s="1"/>
+      <c r="IC75" s="1"/>
+      <c r="ID75" s="1"/>
+      <c r="IE75" s="1"/>
+      <c r="IF75" s="1"/>
+      <c r="IG75" s="1"/>
+      <c r="IH75" s="1"/>
+      <c r="II75" s="1"/>
+      <c r="IJ75" s="1"/>
+      <c r="IK75" s="1"/>
+      <c r="IL75" s="1"/>
+      <c r="IM75" s="1"/>
+      <c r="IN75" s="1"/>
+      <c r="IO75" s="1"/>
+      <c r="IP75" s="1"/>
+      <c r="IQ75" s="1"/>
+      <c r="IR75" s="1"/>
+      <c r="IS75" s="1"/>
+      <c r="IT75" s="1"/>
+      <c r="IU75" s="1"/>
+      <c r="IV75" s="1"/>
+      <c r="IW75" s="1"/>
+      <c r="IX75" s="1"/>
+      <c r="IY75" s="1"/>
+      <c r="IZ75" s="1"/>
+      <c r="JA75" s="1"/>
+      <c r="JB75" s="1"/>
+      <c r="JC75" s="1"/>
+      <c r="JD75" s="1"/>
+      <c r="JE75" s="1"/>
+      <c r="JF75" s="1"/>
+      <c r="JG75" s="1"/>
+      <c r="JH75" s="1"/>
+      <c r="JI75" s="1"/>
+      <c r="JJ75" s="1"/>
+      <c r="JK75" s="1"/>
+      <c r="JL75" s="1"/>
+      <c r="JM75" s="1"/>
+      <c r="JN75" s="1"/>
+      <c r="JO75" s="1"/>
+      <c r="JP75" s="1"/>
+      <c r="JQ75" s="1"/>
+      <c r="JR75" s="1"/>
+      <c r="JS75" s="1"/>
+      <c r="JT75" s="1"/>
+      <c r="JU75" s="1"/>
+      <c r="JV75" s="1"/>
+      <c r="JW75" s="1"/>
+      <c r="JX75" s="1"/>
+      <c r="JY75" s="1"/>
+      <c r="JZ75" s="1"/>
+      <c r="KA75" s="1"/>
+      <c r="KB75" s="1"/>
+      <c r="KC75" s="1"/>
+      <c r="KD75" s="1"/>
+      <c r="KE75" s="1"/>
+      <c r="KF75" s="1"/>
+      <c r="KG75" s="1"/>
+      <c r="KH75" s="1"/>
+      <c r="KI75" s="1"/>
+      <c r="KJ75" s="1"/>
+      <c r="KK75" s="1"/>
+      <c r="KL75" s="1"/>
+      <c r="KM75" s="1"/>
+      <c r="KN75" s="1"/>
+      <c r="KO75" s="1"/>
+      <c r="KP75" s="1"/>
+      <c r="KQ75" s="1"/>
+      <c r="KR75" s="1"/>
+      <c r="KS75" s="1"/>
+      <c r="KT75" s="1"/>
+      <c r="KU75" s="1"/>
+      <c r="KV75" s="1"/>
+      <c r="KW75" s="1"/>
+      <c r="KX75" s="1"/>
+      <c r="KY75" s="1"/>
+      <c r="KZ75" s="1"/>
+      <c r="LA75" s="1"/>
+      <c r="LB75" s="1"/>
+      <c r="LC75" s="1"/>
+      <c r="LD75" s="1"/>
+      <c r="LE75" s="1"/>
+      <c r="LF75" s="1"/>
+      <c r="LG75" s="1"/>
+      <c r="LH75" s="1"/>
+      <c r="LI75" s="1"/>
+      <c r="LJ75" s="1"/>
+      <c r="LK75" s="1"/>
+      <c r="LL75" s="1"/>
+      <c r="LM75" s="1"/>
+      <c r="LN75" s="1"/>
+      <c r="LO75" s="1"/>
+      <c r="LP75" s="1"/>
+      <c r="LQ75" s="1"/>
+      <c r="LR75" s="1"/>
+      <c r="LS75" s="1"/>
+      <c r="LT75" s="1"/>
+      <c r="LU75" s="1"/>
+      <c r="LV75" s="1"/>
+      <c r="LW75" s="1"/>
+      <c r="LX75" s="1"/>
+      <c r="LY75" s="1"/>
+      <c r="LZ75" s="1"/>
+      <c r="MA75" s="1"/>
+      <c r="MB75" s="1"/>
+      <c r="MC75" s="1"/>
+      <c r="MD75" s="1"/>
+      <c r="ME75" s="1"/>
+      <c r="MF75" s="1"/>
+      <c r="MG75" s="1"/>
+      <c r="MH75" s="1"/>
+      <c r="MI75" s="1"/>
+      <c r="MJ75" s="1"/>
+      <c r="MK75" s="1"/>
+      <c r="ML75" s="1"/>
+      <c r="MM75" s="1"/>
+      <c r="MN75" s="1"/>
+      <c r="MO75" s="1"/>
+      <c r="MP75" s="1"/>
+      <c r="MQ75" s="1"/>
+      <c r="MR75" s="1"/>
+      <c r="MS75" s="1"/>
+      <c r="MT75" s="1"/>
+      <c r="MU75" s="1"/>
+      <c r="MV75" s="1"/>
+      <c r="MW75" s="1"/>
+      <c r="MX75" s="1"/>
+      <c r="MY75" s="1"/>
+      <c r="MZ75" s="1"/>
+      <c r="NA75" s="1"/>
+      <c r="NB75" s="1"/>
+      <c r="NC75" s="1"/>
+      <c r="ND75" s="1"/>
+      <c r="NE75" s="1"/>
+      <c r="NF75" s="1"/>
+      <c r="NG75" s="1"/>
+      <c r="NH75" s="1"/>
+      <c r="NI75" s="1"/>
+      <c r="NJ75" s="1"/>
+      <c r="NK75" s="1"/>
+      <c r="NL75" s="1"/>
+      <c r="NM75" s="1"/>
+      <c r="NN75" s="1"/>
+      <c r="NO75" s="1"/>
+      <c r="NP75" s="1"/>
+      <c r="NQ75" s="1"/>
+      <c r="NR75" s="1"/>
+      <c r="NS75" s="1"/>
+      <c r="NT75" s="1"/>
+      <c r="NU75" s="1"/>
+      <c r="NV75" s="1"/>
+      <c r="NW75" s="1"/>
+      <c r="NX75" s="1"/>
+      <c r="NY75" s="1"/>
+      <c r="NZ75" s="1"/>
+      <c r="OA75" s="1"/>
+      <c r="OB75" s="1"/>
+      <c r="OC75" s="1"/>
+      <c r="OD75" s="1"/>
+      <c r="OE75" s="1"/>
+      <c r="OF75" s="1"/>
+      <c r="OG75" s="1"/>
+      <c r="OH75" s="1"/>
+      <c r="OI75" s="1"/>
+      <c r="OJ75" s="1"/>
+      <c r="OK75" s="1"/>
+      <c r="OL75" s="1"/>
+      <c r="OM75" s="1"/>
+      <c r="ON75" s="1"/>
+      <c r="OO75" s="1"/>
+      <c r="OP75" s="1"/>
+      <c r="OQ75" s="1"/>
+      <c r="OR75" s="1"/>
+      <c r="OS75" s="1"/>
+      <c r="OT75" s="1"/>
+      <c r="OU75" s="1"/>
+      <c r="OV75" s="1"/>
+      <c r="OW75" s="1"/>
+      <c r="OX75" s="1"/>
+      <c r="OY75" s="1"/>
+      <c r="OZ75" s="1"/>
+      <c r="PA75" s="1"/>
+      <c r="PB75" s="1"/>
+      <c r="PC75" s="1"/>
+      <c r="PD75" s="1"/>
+      <c r="PE75" s="1"/>
+      <c r="PF75" s="1"/>
+      <c r="PG75" s="1"/>
+      <c r="PH75" s="1"/>
+      <c r="PI75" s="1"/>
+      <c r="PJ75" s="1"/>
+      <c r="PK75" s="1"/>
+      <c r="PL75" s="1"/>
+      <c r="PM75" s="1"/>
+      <c r="PN75" s="1"/>
+      <c r="PO75" s="1"/>
+      <c r="PP75" s="1"/>
+      <c r="PQ75" s="1"/>
+      <c r="PR75" s="1"/>
+      <c r="PS75" s="1"/>
+      <c r="PT75" s="1"/>
+      <c r="PU75" s="1"/>
+      <c r="PV75" s="1"/>
+      <c r="PW75" s="1"/>
+      <c r="PX75" s="1"/>
+      <c r="PY75" s="1"/>
+      <c r="PZ75" s="1"/>
+      <c r="QA75" s="1"/>
+      <c r="QB75" s="1"/>
+      <c r="QC75" s="1"/>
+      <c r="QD75" s="1"/>
+      <c r="QE75" s="1"/>
+      <c r="QF75" s="1"/>
+      <c r="QG75" s="1"/>
+      <c r="QH75" s="1"/>
+      <c r="QI75" s="1"/>
+      <c r="QJ75" s="1"/>
+      <c r="QK75" s="1"/>
+      <c r="QL75" s="1"/>
+      <c r="QM75" s="1"/>
+      <c r="QN75" s="1"/>
+      <c r="QO75" s="1"/>
+      <c r="QP75" s="1"/>
+      <c r="QQ75" s="1"/>
+      <c r="QR75" s="1"/>
+      <c r="QS75" s="1"/>
+      <c r="QT75" s="1"/>
+      <c r="QU75" s="1"/>
+      <c r="QV75" s="1"/>
+      <c r="QW75" s="1"/>
+      <c r="QX75" s="1"/>
+      <c r="QY75" s="1"/>
+      <c r="QZ75" s="1"/>
+      <c r="RA75" s="1"/>
+      <c r="RB75" s="1"/>
+      <c r="RC75" s="1"/>
+      <c r="RD75" s="1"/>
+      <c r="RE75" s="1"/>
+      <c r="RF75" s="1"/>
+      <c r="RG75" s="1"/>
+      <c r="RH75" s="1"/>
+      <c r="RI75" s="1"/>
+      <c r="RJ75" s="1"/>
+      <c r="RK75" s="1"/>
+      <c r="RL75" s="1"/>
+      <c r="RM75" s="1"/>
+      <c r="RN75" s="1"/>
+      <c r="RO75" s="1"/>
+      <c r="RP75" s="1"/>
+      <c r="RQ75" s="1"/>
+      <c r="RR75" s="1"/>
+      <c r="RS75" s="1"/>
+      <c r="RT75" s="1"/>
+      <c r="RU75" s="1"/>
+      <c r="RV75" s="1"/>
+      <c r="RW75" s="1"/>
+      <c r="RX75" s="1"/>
+      <c r="RY75" s="1"/>
+      <c r="RZ75" s="1"/>
+      <c r="SA75" s="1"/>
+      <c r="SB75" s="1"/>
+      <c r="SC75" s="1"/>
+      <c r="SD75" s="1"/>
+      <c r="SE75" s="1"/>
+      <c r="SF75" s="1"/>
+      <c r="SG75" s="1"/>
+      <c r="SH75" s="1"/>
+      <c r="SI75" s="1"/>
+      <c r="SJ75" s="1"/>
+      <c r="SK75" s="1"/>
+      <c r="SL75" s="1"/>
+      <c r="SM75" s="1"/>
+      <c r="SN75" s="1"/>
+      <c r="SO75" s="1"/>
+      <c r="SP75" s="1"/>
+      <c r="SQ75" s="1"/>
+      <c r="SR75" s="1"/>
+      <c r="SS75" s="1"/>
+      <c r="ST75" s="1"/>
+      <c r="SU75" s="1"/>
+      <c r="SV75" s="1"/>
+      <c r="SW75" s="1"/>
+      <c r="SX75" s="1"/>
+      <c r="SY75" s="1"/>
+      <c r="SZ75" s="1"/>
+      <c r="TA75" s="1"/>
+      <c r="TB75" s="1"/>
+      <c r="TC75" s="1"/>
+      <c r="TD75" s="1"/>
+      <c r="TE75" s="1"/>
+      <c r="TF75" s="1"/>
+      <c r="TG75" s="1"/>
+      <c r="TH75" s="1"/>
+      <c r="TI75" s="1"/>
+      <c r="TJ75" s="1"/>
+      <c r="TK75" s="1"/>
+      <c r="TL75" s="1"/>
+      <c r="TM75" s="1"/>
+      <c r="TN75" s="1"/>
+      <c r="TO75" s="1"/>
+      <c r="TP75" s="1"/>
+      <c r="TQ75" s="1"/>
+      <c r="TR75" s="1"/>
+      <c r="TS75" s="1"/>
+      <c r="TT75" s="1"/>
+      <c r="TU75" s="1"/>
+      <c r="TV75" s="1"/>
+      <c r="TW75" s="1"/>
+      <c r="TX75" s="1"/>
+      <c r="TY75" s="1"/>
+      <c r="TZ75" s="1"/>
+      <c r="UA75" s="1"/>
+      <c r="UB75" s="1"/>
+      <c r="UC75" s="1"/>
+      <c r="UD75" s="1"/>
+      <c r="UE75" s="1"/>
+      <c r="UF75" s="1"/>
+      <c r="UG75" s="1"/>
+      <c r="UH75" s="1"/>
+      <c r="UI75" s="1"/>
+      <c r="UJ75" s="1"/>
+      <c r="UK75" s="1"/>
+      <c r="UL75" s="1"/>
+      <c r="UM75" s="1"/>
+      <c r="UN75" s="1"/>
+      <c r="UO75" s="1"/>
+      <c r="UP75" s="1"/>
+      <c r="UQ75" s="1"/>
+      <c r="UR75" s="1"/>
+      <c r="US75" s="1"/>
+      <c r="UT75" s="1"/>
+      <c r="UU75" s="1"/>
+      <c r="UV75" s="1"/>
+      <c r="UW75" s="1"/>
+      <c r="UX75" s="1"/>
+      <c r="UY75" s="1"/>
+      <c r="UZ75" s="1"/>
+      <c r="VA75" s="1"/>
+      <c r="VB75" s="1"/>
+      <c r="VC75" s="1"/>
+      <c r="VD75" s="1"/>
+      <c r="VE75" s="1"/>
+      <c r="VF75" s="1"/>
+      <c r="VG75" s="1"/>
+      <c r="VH75" s="1"/>
+      <c r="VI75" s="1"/>
+      <c r="VJ75" s="1"/>
+      <c r="VK75" s="1"/>
+      <c r="VL75" s="1"/>
+      <c r="VM75" s="1"/>
+      <c r="VN75" s="1"/>
+      <c r="VO75" s="1"/>
+      <c r="VP75" s="1"/>
+      <c r="VQ75" s="1"/>
+      <c r="VR75" s="1"/>
+      <c r="VS75" s="1"/>
+      <c r="VT75" s="1"/>
+      <c r="VU75" s="1"/>
+      <c r="VV75" s="1"/>
+      <c r="VW75" s="1"/>
+      <c r="VX75" s="1"/>
+      <c r="VY75" s="1"/>
+      <c r="VZ75" s="1"/>
+      <c r="WA75" s="1"/>
+      <c r="WB75" s="1"/>
+      <c r="WC75" s="1"/>
+      <c r="WD75" s="1"/>
+      <c r="WE75" s="1"/>
+      <c r="WF75" s="1"/>
+      <c r="WG75" s="1"/>
+      <c r="WH75" s="1"/>
+      <c r="WI75" s="1"/>
+      <c r="WJ75" s="1"/>
+      <c r="WK75" s="1"/>
+      <c r="WL75" s="1"/>
+      <c r="WM75" s="1"/>
+      <c r="WN75" s="1"/>
+      <c r="WO75" s="1"/>
+      <c r="WP75" s="1"/>
+      <c r="WQ75" s="1"/>
+      <c r="WR75" s="1"/>
+      <c r="WS75" s="1"/>
+      <c r="WT75" s="1"/>
+      <c r="WU75" s="1"/>
+      <c r="WV75" s="1"/>
+      <c r="WW75" s="1"/>
+      <c r="WX75" s="1"/>
+      <c r="WY75" s="1"/>
+      <c r="WZ75" s="1"/>
+      <c r="XA75" s="1"/>
+      <c r="XB75" s="1"/>
+      <c r="XC75" s="1"/>
+      <c r="XD75" s="1"/>
+      <c r="XE75" s="1"/>
+      <c r="XF75" s="1"/>
+      <c r="XG75" s="1"/>
+      <c r="XH75" s="1"/>
+      <c r="XI75" s="1"/>
+      <c r="XJ75" s="1"/>
+      <c r="XK75" s="1"/>
+      <c r="XL75" s="1"/>
+      <c r="XM75" s="1"/>
+      <c r="XN75" s="1"/>
+      <c r="XO75" s="1"/>
+      <c r="XP75" s="1"/>
+      <c r="XQ75" s="1"/>
+      <c r="XR75" s="1"/>
+      <c r="XS75" s="1"/>
+      <c r="XT75" s="1"/>
+      <c r="XU75" s="1"/>
+      <c r="XV75" s="1"/>
+      <c r="XW75" s="1"/>
+      <c r="XX75" s="1"/>
+      <c r="XY75" s="1"/>
+      <c r="XZ75" s="1"/>
+      <c r="YA75" s="1"/>
+      <c r="YB75" s="1"/>
+      <c r="YC75" s="1"/>
+      <c r="YD75" s="1"/>
+      <c r="YE75" s="1"/>
+      <c r="YF75" s="1"/>
+      <c r="YG75" s="1"/>
+      <c r="YH75" s="1"/>
+      <c r="YI75" s="1"/>
+      <c r="YJ75" s="1"/>
+      <c r="YK75" s="1"/>
+      <c r="YL75" s="1"/>
+      <c r="YM75" s="1"/>
+      <c r="YN75" s="1"/>
+      <c r="YO75" s="1"/>
+      <c r="YP75" s="1"/>
+      <c r="YQ75" s="1"/>
+      <c r="YR75" s="1"/>
+      <c r="YS75" s="1"/>
+      <c r="YT75" s="1"/>
+      <c r="YU75" s="1"/>
+      <c r="YV75" s="1"/>
+      <c r="YW75" s="1"/>
+      <c r="YX75" s="1"/>
+      <c r="YY75" s="1"/>
+      <c r="YZ75" s="1"/>
+      <c r="ZA75" s="1"/>
+      <c r="ZB75" s="1"/>
+      <c r="ZC75" s="1"/>
+      <c r="ZD75" s="1"/>
+      <c r="ZE75" s="1"/>
+      <c r="ZF75" s="1"/>
+      <c r="ZG75" s="1"/>
+      <c r="ZH75" s="1"/>
+      <c r="ZI75" s="1"/>
+      <c r="ZJ75" s="1"/>
+      <c r="ZK75" s="1"/>
+      <c r="ZL75" s="1"/>
+      <c r="ZM75" s="1"/>
+      <c r="ZN75" s="1"/>
+      <c r="ZO75" s="1"/>
+      <c r="ZP75" s="1"/>
+      <c r="ZQ75" s="1"/>
+      <c r="ZR75" s="1"/>
+      <c r="ZS75" s="1"/>
+      <c r="ZT75" s="1"/>
+      <c r="ZU75" s="1"/>
+      <c r="ZV75" s="1"/>
+      <c r="ZW75" s="1"/>
+      <c r="ZX75" s="1"/>
+      <c r="ZY75" s="1"/>
+      <c r="ZZ75" s="1"/>
+      <c r="AAA75" s="1"/>
+      <c r="AAB75" s="1"/>
+      <c r="AAC75" s="1"/>
+      <c r="AAD75" s="1"/>
+      <c r="AAE75" s="1"/>
+      <c r="AAF75" s="1"/>
+      <c r="AAG75" s="1"/>
+      <c r="AAH75" s="1"/>
+      <c r="AAI75" s="1"/>
+      <c r="AAJ75" s="1"/>
+      <c r="AAK75" s="1"/>
+      <c r="AAL75" s="1"/>
+      <c r="AAM75" s="1"/>
+      <c r="AAN75" s="1"/>
+      <c r="AAO75" s="1"/>
+      <c r="AAP75" s="1"/>
+      <c r="AAQ75" s="1"/>
+      <c r="AAR75" s="1"/>
+      <c r="AAS75" s="1"/>
+      <c r="AAT75" s="1"/>
+      <c r="AAU75" s="1"/>
+      <c r="AAV75" s="1"/>
+      <c r="AAW75" s="1"/>
+      <c r="AAX75" s="1"/>
+      <c r="AAY75" s="1"/>
+      <c r="AAZ75" s="1"/>
+      <c r="ABA75" s="1"/>
+      <c r="ABB75" s="1"/>
+      <c r="ABC75" s="1"/>
+      <c r="ABD75" s="1"/>
+      <c r="ABE75" s="1"/>
+      <c r="ABF75" s="1"/>
+      <c r="ABG75" s="1"/>
+      <c r="ABH75" s="1"/>
+      <c r="ABI75" s="1"/>
+      <c r="ABJ75" s="1"/>
+      <c r="ABK75" s="1"/>
+      <c r="ABL75" s="1"/>
+      <c r="ABM75" s="1"/>
+      <c r="ABN75" s="1"/>
+      <c r="ABO75" s="1"/>
+      <c r="ABP75" s="1"/>
+      <c r="ABQ75" s="1"/>
+      <c r="ABR75" s="1"/>
+      <c r="ABS75" s="1"/>
+      <c r="ABT75" s="1"/>
+      <c r="ABU75" s="1"/>
+      <c r="ABV75" s="1"/>
+      <c r="ABW75" s="1"/>
+      <c r="ABX75" s="1"/>
+      <c r="ABY75" s="1"/>
+      <c r="ABZ75" s="1"/>
+      <c r="ACA75" s="1"/>
+      <c r="ACB75" s="1"/>
+      <c r="ACC75" s="1"/>
+      <c r="ACD75" s="1"/>
+      <c r="ACE75" s="1"/>
+      <c r="ACF75" s="1"/>
+      <c r="ACG75" s="1"/>
+      <c r="ACH75" s="1"/>
+      <c r="ACI75" s="1"/>
+      <c r="ACJ75" s="1"/>
+      <c r="ACK75" s="1"/>
+      <c r="ACL75" s="1"/>
+      <c r="ACM75" s="1"/>
+      <c r="ACN75" s="1"/>
+      <c r="ACO75" s="1"/>
+      <c r="ACP75" s="1"/>
+      <c r="ACQ75" s="1"/>
+      <c r="ACR75" s="1"/>
+      <c r="ACS75" s="1"/>
+      <c r="ACT75" s="1"/>
+      <c r="ACU75" s="1"/>
+      <c r="ACV75" s="1"/>
+      <c r="ACW75" s="1"/>
+      <c r="ACX75" s="1"/>
+      <c r="ACY75" s="1"/>
+      <c r="ACZ75" s="1"/>
+      <c r="ADA75" s="1"/>
+      <c r="ADB75" s="1"/>
+      <c r="ADC75" s="1"/>
+      <c r="ADD75" s="1"/>
+      <c r="ADE75" s="1"/>
+      <c r="ADF75" s="1"/>
+      <c r="ADG75" s="1"/>
+      <c r="ADH75" s="1"/>
+      <c r="ADI75" s="1"/>
+      <c r="ADJ75" s="1"/>
+      <c r="ADK75" s="1"/>
+      <c r="ADL75" s="1"/>
+      <c r="ADM75" s="1"/>
+      <c r="ADN75" s="1"/>
+      <c r="ADO75" s="1"/>
+      <c r="ADP75" s="1"/>
+      <c r="ADQ75" s="1"/>
+      <c r="ADR75" s="1"/>
+      <c r="ADS75" s="1"/>
+      <c r="ADT75" s="1"/>
+      <c r="ADU75" s="1"/>
+      <c r="ADV75" s="1"/>
+      <c r="ADW75" s="1"/>
+      <c r="ADX75" s="1"/>
+      <c r="ADY75" s="1"/>
+      <c r="ADZ75" s="1"/>
+      <c r="AEA75" s="1"/>
+      <c r="AEB75" s="1"/>
+      <c r="AEC75" s="1"/>
+      <c r="AED75" s="1"/>
+      <c r="AEE75" s="1"/>
+      <c r="AEF75" s="1"/>
+      <c r="AEG75" s="1"/>
+      <c r="AEH75" s="1"/>
+      <c r="AEI75" s="1"/>
+      <c r="AEJ75" s="1"/>
+      <c r="AEK75" s="1"/>
+      <c r="AEL75" s="1"/>
+      <c r="AEM75" s="1"/>
+      <c r="AEN75" s="1"/>
+      <c r="AEO75" s="1"/>
+      <c r="AEP75" s="1"/>
+      <c r="AEQ75" s="1"/>
+      <c r="AER75" s="1"/>
+      <c r="AES75" s="1"/>
+      <c r="AET75" s="1"/>
+      <c r="AEU75" s="1"/>
+      <c r="AEV75" s="1"/>
+      <c r="AEW75" s="1"/>
+      <c r="AEX75" s="1"/>
+      <c r="AEY75" s="1"/>
+      <c r="AEZ75" s="1"/>
+      <c r="AFA75" s="1"/>
+      <c r="AFB75" s="1"/>
+      <c r="AFC75" s="1"/>
+      <c r="AFD75" s="1"/>
+      <c r="AFE75" s="1"/>
+      <c r="AFF75" s="1"/>
+      <c r="AFG75" s="1"/>
+      <c r="AFH75" s="1"/>
+      <c r="AFI75" s="1"/>
+      <c r="AFJ75" s="1"/>
+      <c r="AFK75" s="1"/>
+      <c r="AFL75" s="1"/>
+      <c r="AFM75" s="1"/>
+      <c r="AFN75" s="1"/>
+      <c r="AFO75" s="1"/>
+      <c r="AFP75" s="1"/>
+      <c r="AFQ75" s="1"/>
+      <c r="AFR75" s="1"/>
+      <c r="AFS75" s="1"/>
+      <c r="AFT75" s="1"/>
+      <c r="AFU75" s="1"/>
+      <c r="AFV75" s="1"/>
+      <c r="AFW75" s="1"/>
+      <c r="AFX75" s="1"/>
+      <c r="AFY75" s="1"/>
+      <c r="AFZ75" s="1"/>
+      <c r="AGA75" s="1"/>
+      <c r="AGB75" s="1"/>
+      <c r="AGC75" s="1"/>
+      <c r="AGD75" s="1"/>
+      <c r="AGE75" s="1"/>
+      <c r="AGF75" s="1"/>
+      <c r="AGG75" s="1"/>
+      <c r="AGH75" s="1"/>
+      <c r="AGI75" s="1"/>
+      <c r="AGJ75" s="1"/>
+      <c r="AGK75" s="1"/>
+      <c r="AGL75" s="1"/>
+      <c r="AGM75" s="1"/>
+      <c r="AGN75" s="1"/>
+      <c r="AGO75" s="1"/>
+      <c r="AGP75" s="1"/>
+      <c r="AGQ75" s="1"/>
+      <c r="AGR75" s="1"/>
+      <c r="AGS75" s="1"/>
+      <c r="AGT75" s="1"/>
+      <c r="AGU75" s="1"/>
+      <c r="AGV75" s="1"/>
+      <c r="AGW75" s="1"/>
+      <c r="AGX75" s="1"/>
+      <c r="AGY75" s="1"/>
+      <c r="AGZ75" s="1"/>
+      <c r="AHA75" s="1"/>
+      <c r="AHB75" s="1"/>
+      <c r="AHC75" s="1"/>
+      <c r="AHD75" s="1"/>
+      <c r="AHE75" s="1"/>
+      <c r="AHF75" s="1"/>
+      <c r="AHG75" s="1"/>
+      <c r="AHH75" s="1"/>
+      <c r="AHI75" s="1"/>
+      <c r="AHJ75" s="1"/>
+      <c r="AHK75" s="1"/>
+      <c r="AHL75" s="1"/>
+      <c r="AHM75" s="1"/>
+      <c r="AHN75" s="1"/>
+      <c r="AHO75" s="1"/>
+      <c r="AHP75" s="1"/>
+      <c r="AHQ75" s="1"/>
+      <c r="AHR75" s="1"/>
+      <c r="AHS75" s="1"/>
+      <c r="AHT75" s="1"/>
+      <c r="AHU75" s="1"/>
+      <c r="AHV75" s="1"/>
+      <c r="AHW75" s="1"/>
+      <c r="AHX75" s="1"/>
+      <c r="AHY75" s="1"/>
+      <c r="AHZ75" s="1"/>
+      <c r="AIA75" s="1"/>
+      <c r="AIB75" s="1"/>
+      <c r="AIC75" s="1"/>
+      <c r="AID75" s="1"/>
+      <c r="AIE75" s="1"/>
+      <c r="AIF75" s="1"/>
+      <c r="AIG75" s="1"/>
+      <c r="AIH75" s="1"/>
+      <c r="AII75" s="1"/>
+      <c r="AIJ75" s="1"/>
+      <c r="AIK75" s="1"/>
+      <c r="AIL75" s="1"/>
+      <c r="AIM75" s="1"/>
+      <c r="AIN75" s="1"/>
+      <c r="AIO75" s="1"/>
+      <c r="AIP75" s="1"/>
+      <c r="AIQ75" s="1"/>
+      <c r="AIR75" s="1"/>
+      <c r="AIS75" s="1"/>
+      <c r="AIT75" s="1"/>
+      <c r="AIU75" s="1"/>
+      <c r="AIV75" s="1"/>
+      <c r="AIW75" s="1"/>
+      <c r="AIX75" s="1"/>
+      <c r="AIY75" s="1"/>
+      <c r="AIZ75" s="1"/>
+      <c r="AJA75" s="1"/>
+      <c r="AJB75" s="1"/>
+      <c r="AJC75" s="1"/>
+      <c r="AJD75" s="1"/>
+      <c r="AJE75" s="1"/>
+      <c r="AJF75" s="1"/>
+      <c r="AJG75" s="1"/>
+      <c r="AJH75" s="1"/>
+      <c r="AJI75" s="1"/>
+      <c r="AJJ75" s="1"/>
+      <c r="AJK75" s="1"/>
+      <c r="AJL75" s="1"/>
+      <c r="AJM75" s="1"/>
+      <c r="AJN75" s="1"/>
+      <c r="AJO75" s="1"/>
+      <c r="AJP75" s="1"/>
+      <c r="AJQ75" s="1"/>
+      <c r="AJR75" s="1"/>
+      <c r="AJS75" s="1"/>
+      <c r="AJT75" s="1"/>
+      <c r="AJU75" s="1"/>
+      <c r="AJV75" s="1"/>
+      <c r="AJW75" s="1"/>
+      <c r="AJX75" s="1"/>
+      <c r="AJY75" s="1"/>
+      <c r="AJZ75" s="1"/>
+      <c r="AKA75" s="1"/>
+      <c r="AKB75" s="1"/>
+      <c r="AKC75" s="1"/>
+      <c r="AKD75" s="1"/>
+      <c r="AKE75" s="1"/>
+      <c r="AKF75" s="1"/>
+      <c r="AKG75" s="1"/>
+      <c r="AKH75" s="1"/>
+      <c r="AKI75" s="1"/>
+      <c r="AKJ75" s="1"/>
+      <c r="AKK75" s="1"/>
+      <c r="AKL75" s="1"/>
+      <c r="AKM75" s="1"/>
+      <c r="AKN75" s="1"/>
+      <c r="AKO75" s="1"/>
+      <c r="AKP75" s="1"/>
+      <c r="AKQ75" s="1"/>
+      <c r="AKR75" s="1"/>
+      <c r="AKS75" s="1"/>
+      <c r="AKT75" s="1"/>
+      <c r="AKU75" s="1"/>
+      <c r="AKV75" s="1"/>
+      <c r="AKW75" s="1"/>
+      <c r="AKX75" s="1"/>
+      <c r="AKY75" s="1"/>
+      <c r="AKZ75" s="1"/>
+      <c r="ALA75" s="1"/>
+      <c r="ALB75" s="1"/>
+      <c r="ALC75" s="1"/>
+      <c r="ALD75" s="1"/>
+      <c r="ALE75" s="1"/>
+      <c r="ALF75" s="1"/>
+      <c r="ALG75" s="1"/>
+      <c r="ALH75" s="1"/>
+      <c r="ALI75" s="1"/>
+      <c r="ALJ75" s="1"/>
+      <c r="ALK75" s="1"/>
+      <c r="ALL75" s="1"/>
+      <c r="ALM75" s="1"/>
+      <c r="ALN75" s="1"/>
+      <c r="ALO75" s="1"/>
+      <c r="ALP75" s="1"/>
+      <c r="ALQ75" s="1"/>
+      <c r="ALR75" s="1"/>
+      <c r="ALS75" s="1"/>
+      <c r="ALT75" s="1"/>
+      <c r="ALU75" s="1"/>
+      <c r="ALV75" s="1"/>
+      <c r="ALW75" s="1"/>
+      <c r="ALX75" s="1"/>
+      <c r="ALY75" s="1"/>
+      <c r="ALZ75" s="1"/>
+      <c r="AMA75" s="1"/>
+      <c r="AMB75" s="1"/>
+      <c r="AMC75" s="1"/>
+      <c r="AMD75" s="1"/>
+      <c r="AME75" s="1"/>
+      <c r="AMF75" s="1"/>
+      <c r="AMG75" s="1"/>
+      <c r="AMH75" s="1"/>
+      <c r="AMI75" s="1"/>
+      <c r="AMJ75" s="1"/>
+      <c r="AMK75" s="1"/>
+    </row>
+    <row r="76" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B76" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C76" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A77" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C77" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C78" s="5" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A79" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C79" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:1025" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C80" s="4" t="s">
         <v>235</v>
       </c>
     </row>
+    <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A83" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A84" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A86" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A87" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A88" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A2:AMK2" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AMK88">
+      <sortCondition ref="A2"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C72">
     <sortCondition ref="A3:A72"/>
   </sortState>
@@ -2162,83 +4384,112 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C62" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C30" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C17" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C18" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C70" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C23" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C67" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C64" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C31" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C33" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C37" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C36" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C42" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C43" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C47" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C40" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C44" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C39" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C51" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C53" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C55" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C58" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C57" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C15" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C68" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C61" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C71" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C72" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C65" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C41" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C35" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C63" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C5" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C38" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C49" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C73" r:id="rId51" xr:uid="{D4EC3F26-FB9B-0C4C-A9BF-D5766209B760}"/>
-    <hyperlink ref="C74" r:id="rId52" xr:uid="{4FBF0906-9AF5-D142-B9D1-1BEF3B0A1FEE}"/>
-    <hyperlink ref="C75" r:id="rId53" xr:uid="{0D9565FC-23CE-7743-ADFA-9A087B7C25D3}"/>
-    <hyperlink ref="C76" r:id="rId54" xr:uid="{47453487-DE29-E249-95B5-E46513555F55}"/>
-    <hyperlink ref="C77" r:id="rId55" xr:uid="{D034833B-B5AE-614C-B976-B8F12F8AB280}"/>
-    <hyperlink ref="C78" r:id="rId56" xr:uid="{D069C9A5-D5AC-0B46-A34E-B50258C56053}"/>
-    <hyperlink ref="C79" r:id="rId57" xr:uid="{BE3AC031-8C70-9C41-8DC7-88700E8C32CA}"/>
-    <hyperlink ref="C66" r:id="rId58" xr:uid="{DF192853-BCD5-E947-A105-44BE7CB5CF72}"/>
-    <hyperlink ref="C7" r:id="rId59" xr:uid="{470CBD7E-33DA-4B21-B8E2-B4245DC824F9}"/>
-    <hyperlink ref="C32" r:id="rId60" xr:uid="{6D3F7EC2-6E99-4830-BFBD-AF4938F90032}"/>
-    <hyperlink ref="C34" r:id="rId61" xr:uid="{A5049810-F177-4DB3-8129-6A0BCC790164}"/>
-    <hyperlink ref="C8" r:id="rId62" xr:uid="{AC0D0AB7-0BC3-4F09-BDD1-2E7C15FC0C4F}"/>
-    <hyperlink ref="C59" r:id="rId63" xr:uid="{5259C5DB-4130-4B45-97CA-D23E8CE07F78}"/>
-    <hyperlink ref="C54" r:id="rId64" xr:uid="{A61A251B-14DB-4690-AC31-7A1836680CF3}"/>
-    <hyperlink ref="C60" r:id="rId65" xr:uid="{58614A08-2023-451C-9C66-88C2FD08E9AE}"/>
-    <hyperlink ref="C9" r:id="rId66" xr:uid="{A374CCDF-5F4A-4B09-B50F-80F234168E91}"/>
-    <hyperlink ref="C50" r:id="rId67" xr:uid="{941F840C-1B87-4863-A9DA-679DE419CC00}"/>
-    <hyperlink ref="C69" r:id="rId68" xr:uid="{3A7EB2C3-4F2B-4CBC-BB56-FE1E9592C8AC}"/>
-    <hyperlink ref="C6" r:id="rId69" xr:uid="{E3974922-3343-4172-9DB2-75C9DC76E6EF}"/>
+    <hyperlink ref="C77" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C36" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C21" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C24" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C25" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C86" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C26" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C83" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C34" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C79" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C40" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C42" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C49" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C47" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C55" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C56" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C60" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C53" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C57" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C52" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C59" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C65" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C67" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C69" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C72" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C71" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C17" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C84" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C76" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C87" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C88" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C80" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C54" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C46" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C61" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C78" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C6" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C50" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C62" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C44" r:id="rId52" xr:uid="{D4EC3F26-FB9B-0C4C-A9BF-D5766209B760}"/>
+    <hyperlink ref="C43" r:id="rId53" xr:uid="{4FBF0906-9AF5-D142-B9D1-1BEF3B0A1FEE}"/>
+    <hyperlink ref="C38" r:id="rId54" xr:uid="{0D9565FC-23CE-7743-ADFA-9A087B7C25D3}"/>
+    <hyperlink ref="C63" r:id="rId55" xr:uid="{47453487-DE29-E249-95B5-E46513555F55}"/>
+    <hyperlink ref="C13" r:id="rId56" xr:uid="{D034833B-B5AE-614C-B976-B8F12F8AB280}"/>
+    <hyperlink ref="C48" r:id="rId57" xr:uid="{D069C9A5-D5AC-0B46-A34E-B50258C56053}"/>
+    <hyperlink ref="C35" r:id="rId58" xr:uid="{BE3AC031-8C70-9C41-8DC7-88700E8C32CA}"/>
+    <hyperlink ref="C82" r:id="rId59" xr:uid="{DF192853-BCD5-E947-A105-44BE7CB5CF72}"/>
+    <hyperlink ref="C9" r:id="rId60" xr:uid="{470CBD7E-33DA-4B21-B8E2-B4245DC824F9}"/>
+    <hyperlink ref="C41" r:id="rId61" xr:uid="{6D3F7EC2-6E99-4830-BFBD-AF4938F90032}"/>
+    <hyperlink ref="C45" r:id="rId62" xr:uid="{A5049810-F177-4DB3-8129-6A0BCC790164}"/>
+    <hyperlink ref="C8" r:id="rId63" xr:uid="{AC0D0AB7-0BC3-4F09-BDD1-2E7C15FC0C4F}"/>
+    <hyperlink ref="C74" r:id="rId64" xr:uid="{5259C5DB-4130-4B45-97CA-D23E8CE07F78}"/>
+    <hyperlink ref="C68" r:id="rId65" xr:uid="{A61A251B-14DB-4690-AC31-7A1836680CF3}"/>
+    <hyperlink ref="C75" r:id="rId66" xr:uid="{58614A08-2023-451C-9C66-88C2FD08E9AE}"/>
+    <hyperlink ref="C10" r:id="rId67" xr:uid="{A374CCDF-5F4A-4B09-B50F-80F234168E91}"/>
+    <hyperlink ref="C64" r:id="rId68" xr:uid="{941F840C-1B87-4863-A9DA-679DE419CC00}"/>
+    <hyperlink ref="C85" r:id="rId69" xr:uid="{93DEF860-006B-4E3A-A816-38C1C82D6317}"/>
+    <hyperlink ref="C19" r:id="rId70" xr:uid="{62BCF645-6D80-45DD-9343-FA35666B2386}"/>
+    <hyperlink ref="C81" r:id="rId71" xr:uid="{44093101-D604-4123-B604-6D76F1372904}"/>
+    <hyperlink ref="C5" r:id="rId72" xr:uid="{85FD52CC-1713-4C06-811D-09AD3316E198}"/>
+    <hyperlink ref="C39" r:id="rId73" xr:uid="{E18060C8-5946-4506-B18C-C9DC32A0271E}"/>
+    <hyperlink ref="C29" r:id="rId74" xr:uid="{F8B8A102-D577-4144-850C-62AA613800D2}"/>
+    <hyperlink ref="C27" r:id="rId75" xr:uid="{4B4E53D5-A82D-4617-B626-7A7300AD42C4}"/>
+    <hyperlink ref="C37" r:id="rId76" xr:uid="{D0E329FD-F3D0-4ED3-A906-718DAF5A8472}"/>
+    <hyperlink ref="C73" r:id="rId77" xr:uid="{DA5B1321-3236-4A2E-A220-6451ED8BF8AA}"/>
+    <hyperlink ref="C51" r:id="rId78" xr:uid="{82FE7554-A447-4220-B9C3-DC31EA1E73E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId70"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId79"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006651BF32B521A046AF14BF632D6B295F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="09153fd41ce1666f2d769619857e3bdc">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67f489d-6419-4cb0-8238-506a3a8f1300" xmlns:ns3="0ce01a67-a604-4be1-a4ca-c8b766b5a068" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="de1bb72c62ccf761f278c18d78bd3734" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b67f489d-6419-4cb0-8238-506a3a8f1300">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0ce01a67-a604-4be1-a4ca-c8b766b5a068" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006651BF32B521A046AF14BF632D6B295F" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="55423843e2650ade946de227fdfd3c86">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67f489d-6419-4cb0-8238-506a3a8f1300" xmlns:ns3="0ce01a67-a604-4be1-a4ca-c8b766b5a068" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b15cf6a4d7b0b7ca33e0fb73ec1791d3" ns2:_="" ns3:_="">
     <xsd:import namespace="b67f489d-6419-4cb0-8238-506a3a8f1300"/>
     <xsd:import namespace="0ce01a67-a604-4be1-a4ca-c8b766b5a068"/>
     <xsd:element name="properties">
@@ -2257,6 +4508,9 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2316,6 +4570,11 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0ce01a67-a604-4be1-a4ca-c8b766b5a068" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2330,6 +4589,32 @@
           </xsd:extension>
         </xsd:complexContent>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -2431,34 +4716,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b67f489d-6419-4cb0-8238-506a3a8f1300">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0ce01a67-a604-4be1-a4ca-c8b766b5a068" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DCBA043-5AC9-4F81-BC42-453A12F56987}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2792C375-D0AA-48DB-A092-AE38FD1E93C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b67f489d-6419-4cb0-8238-506a3a8f1300"/>
+    <ds:schemaRef ds:uri="0ce01a67-a604-4be1-a4ca-c8b766b5a068"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B72C46E4-6E94-400B-A21B-130440CD1956}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C149E5CF-E330-427D-9820-2F7DEFB0B68C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3AC60EA-A07C-4B41-826E-3D51559D0E0D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1B05E73-26DD-4B88-B2EA-BF03046236C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b67f489d-6419-4cb0-8238-506a3a8f1300"/>
+    <ds:schemaRef ds:uri="0ce01a67-a604-4be1-a4ca-c8b766b5a068"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>